<commit_message>
Added SVM model for whole data
</commit_message>
<xml_diff>
--- a/BlueChannel.xlsx
+++ b/BlueChannel.xlsx
@@ -423,47 +423,47 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>MeanB</t>
+          <t>Mean_B</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>VarianceB</t>
+          <t>Variance_B</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>SkewnessB</t>
+          <t>Skewness_B</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>KurtosisB</t>
+          <t>Kurtosis_B</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>ContrastB</t>
+          <t>Contrast_B</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>EntropyB</t>
+          <t>Entropy_B</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>EnergyB</t>
+          <t>Energy_B</t>
         </is>
       </c>
       <c r="H1" t="inlineStr">
         <is>
-          <t>HomoB</t>
+          <t>Homogeneity_B</t>
         </is>
       </c>
       <c r="I1" t="inlineStr">
         <is>
-          <t>CorreB</t>
+          <t>Correlation_B</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Added Smoothness for all the images
</commit_message>
<xml_diff>
--- a/BlueChannel.xlsx
+++ b/BlueChannel.xlsx
@@ -412,7 +412,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L301"/>
+  <dimension ref="A1:N301"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -481,6 +481,16 @@
           <t>Correlation_B</t>
         </is>
       </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>IDM_B</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>Smoothness_B</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -519,6 +529,12 @@
       <c r="L2" t="n">
         <v>0.8509681817418654</v>
       </c>
+      <c r="M2" t="n">
+        <v>0.001205584601949051</v>
+      </c>
+      <c r="N2" t="n">
+        <v>0.0126411209218469</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
@@ -557,6 +573,12 @@
       <c r="L3" t="n">
         <v>0.8306198855451331</v>
       </c>
+      <c r="M3" t="n">
+        <v>0.001201981418488809</v>
+      </c>
+      <c r="N3" t="n">
+        <v>0.012679581458579</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
@@ -595,6 +617,12 @@
       <c r="L4" t="n">
         <v>0.7944726218972304</v>
       </c>
+      <c r="M4" t="n">
+        <v>0.0009088575901376786</v>
+      </c>
+      <c r="N4" t="n">
+        <v>0.01677381621191392</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
@@ -633,6 +661,12 @@
       <c r="L5" t="n">
         <v>0.8947472586582648</v>
       </c>
+      <c r="M5" t="n">
+        <v>0.001764372951388545</v>
+      </c>
+      <c r="N5" t="n">
+        <v>0.008632527163699097</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
@@ -671,6 +705,12 @@
       <c r="L6" t="n">
         <v>0.9212388936559259</v>
       </c>
+      <c r="M6" t="n">
+        <v>0.001650590637034887</v>
+      </c>
+      <c r="N6" t="n">
+        <v>0.009229177224397178</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
@@ -709,6 +749,12 @@
       <c r="L7" t="n">
         <v>0.8869762914494788</v>
       </c>
+      <c r="M7" t="n">
+        <v>0.001684670017583568</v>
+      </c>
+      <c r="N7" t="n">
+        <v>0.009042211318648533</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
@@ -747,6 +793,12 @@
       <c r="L8" t="n">
         <v>0.9070151882863146</v>
       </c>
+      <c r="M8" t="n">
+        <v>0.001999183096652939</v>
+      </c>
+      <c r="N8" t="n">
+        <v>0.007617287127578955</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
@@ -785,6 +837,12 @@
       <c r="L9" t="n">
         <v>0.8987688911999009</v>
       </c>
+      <c r="M9" t="n">
+        <v>0.008765499279158854</v>
+      </c>
+      <c r="N9" t="n">
+        <v>0.001725789172412317</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
@@ -823,6 +881,12 @@
       <c r="L10" t="n">
         <v>0.8342181041067811</v>
       </c>
+      <c r="M10" t="n">
+        <v>0.001560775179904465</v>
+      </c>
+      <c r="N10" t="n">
+        <v>0.009761061195179575</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
@@ -861,6 +925,12 @@
       <c r="L11" t="n">
         <v>0.6633297817966149</v>
       </c>
+      <c r="M11" t="n">
+        <v>0.000725635264958599</v>
+      </c>
+      <c r="N11" t="n">
+        <v>0.02101304752052529</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
@@ -899,6 +969,12 @@
       <c r="L12" t="n">
         <v>0.871844178495586</v>
       </c>
+      <c r="M12" t="n">
+        <v>0.001704291488109693</v>
+      </c>
+      <c r="N12" t="n">
+        <v>0.008937499686081632</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
@@ -937,6 +1013,12 @@
       <c r="L13" t="n">
         <v>0.5103184433968952</v>
       </c>
+      <c r="M13" t="n">
+        <v>0.0004520434897256011</v>
+      </c>
+      <c r="N13" t="n">
+        <v>0.03373987647758131</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
@@ -975,6 +1057,12 @@
       <c r="L14" t="n">
         <v>0.8580670131431076</v>
       </c>
+      <c r="M14" t="n">
+        <v>0.0008733481552575101</v>
+      </c>
+      <c r="N14" t="n">
+        <v>0.01745619978274476</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
@@ -1013,6 +1101,12 @@
       <c r="L15" t="n">
         <v>0.7419795479988743</v>
       </c>
+      <c r="M15" t="n">
+        <v>0.0007965947138359853</v>
+      </c>
+      <c r="N15" t="n">
+        <v>0.01913989327183034</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
@@ -1051,6 +1145,12 @@
       <c r="L16" t="n">
         <v>0.8937005531700279</v>
       </c>
+      <c r="M16" t="n">
+        <v>0.001156547040189623</v>
+      </c>
+      <c r="N16" t="n">
+        <v>0.01317580350900269</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
@@ -1089,6 +1189,12 @@
       <c r="L17" t="n">
         <v>0.9859079658223292</v>
       </c>
+      <c r="M17" t="n">
+        <v>0.02098488915610815</v>
+      </c>
+      <c r="N17" t="n">
+        <v>0.0007122874589939842</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
@@ -1127,6 +1233,12 @@
       <c r="L18" t="n">
         <v>0.7346527927508443</v>
       </c>
+      <c r="M18" t="n">
+        <v>0.0005988442014260956</v>
+      </c>
+      <c r="N18" t="n">
+        <v>0.02546478077448096</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
@@ -1165,6 +1277,12 @@
       <c r="L19" t="n">
         <v>0.9949869517976108</v>
       </c>
+      <c r="M19" t="n">
+        <v>0.03206271720892582</v>
+      </c>
+      <c r="N19" t="n">
+        <v>0.0004606146710541318</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
@@ -1203,6 +1321,12 @@
       <c r="L20" t="n">
         <v>0.8550955564332295</v>
       </c>
+      <c r="M20" t="n">
+        <v>0.0006409391151856374</v>
+      </c>
+      <c r="N20" t="n">
+        <v>0.02379377849055945</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
@@ -1241,6 +1365,12 @@
       <c r="L21" t="n">
         <v>0.9736957536362507</v>
       </c>
+      <c r="M21" t="n">
+        <v>0.01158961766371981</v>
+      </c>
+      <c r="N21" t="n">
+        <v>0.001301660903445555</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
@@ -1279,6 +1409,12 @@
       <c r="L22" t="n">
         <v>0.8853769615431825</v>
       </c>
+      <c r="M22" t="n">
+        <v>0.001346170451786427</v>
+      </c>
+      <c r="N22" t="n">
+        <v>0.01131945056657807</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
@@ -1317,6 +1453,12 @@
       <c r="L23" t="n">
         <v>0.6910599784944554</v>
       </c>
+      <c r="M23" t="n">
+        <v>0.0005664359527299282</v>
+      </c>
+      <c r="N23" t="n">
+        <v>0.02692310956660164</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
@@ -1355,6 +1497,12 @@
       <c r="L24" t="n">
         <v>0.9224580843435668</v>
       </c>
+      <c r="M24" t="n">
+        <v>0.00171792906862542</v>
+      </c>
+      <c r="N24" t="n">
+        <v>0.008866347658853605</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
@@ -1393,6 +1541,12 @@
       <c r="L25" t="n">
         <v>0.8911402659860364</v>
       </c>
+      <c r="M25" t="n">
+        <v>0.001806020187465741</v>
+      </c>
+      <c r="N25" t="n">
+        <v>0.008435492137015891</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
@@ -1431,6 +1585,12 @@
       <c r="L26" t="n">
         <v>0.9116742863449039</v>
       </c>
+      <c r="M26" t="n">
+        <v>0.00306598566077075</v>
+      </c>
+      <c r="N26" t="n">
+        <v>0.004961907512987063</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
@@ -1469,6 +1629,12 @@
       <c r="L27" t="n">
         <v>0.8924777393832696</v>
       </c>
+      <c r="M27" t="n">
+        <v>0.001959196876022527</v>
+      </c>
+      <c r="N27" t="n">
+        <v>0.007773161649199826</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
@@ -1507,6 +1673,12 @@
       <c r="L28" t="n">
         <v>0.9780791635980135</v>
       </c>
+      <c r="M28" t="n">
+        <v>0.00884250284009634</v>
+      </c>
+      <c r="N28" t="n">
+        <v>0.001709635700401733</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
@@ -1545,6 +1717,12 @@
       <c r="L29" t="n">
         <v>0.7849317330854523</v>
       </c>
+      <c r="M29" t="n">
+        <v>0.001055964482517004</v>
+      </c>
+      <c r="N29" t="n">
+        <v>0.01443497549522967</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
@@ -1583,6 +1761,12 @@
       <c r="L30" t="n">
         <v>0.8302295296782917</v>
       </c>
+      <c r="M30" t="n">
+        <v>0.001077800898401972</v>
+      </c>
+      <c r="N30" t="n">
+        <v>0.01414149430933846</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
@@ -1621,6 +1805,12 @@
       <c r="L31" t="n">
         <v>0.6268336562207085</v>
       </c>
+      <c r="M31" t="n">
+        <v>0.0004589361861378425</v>
+      </c>
+      <c r="N31" t="n">
+        <v>0.03323278761067797</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="n">
@@ -1659,6 +1849,12 @@
       <c r="L32" t="n">
         <v>0.9037078168927269</v>
       </c>
+      <c r="M32" t="n">
+        <v>0.001715595288242975</v>
+      </c>
+      <c r="N32" t="n">
+        <v>0.008878934637703194</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="n">
@@ -1697,6 +1893,12 @@
       <c r="L33" t="n">
         <v>0.9952448838967668</v>
       </c>
+      <c r="M33" t="n">
+        <v>0.07046158475173896</v>
+      </c>
+      <c r="N33" t="n">
+        <v>0.0002019835384086387</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="n">
@@ -1735,6 +1937,12 @@
       <c r="L34" t="n">
         <v>0.6975840606655895</v>
       </c>
+      <c r="M34" t="n">
+        <v>0.0005549011527225559</v>
+      </c>
+      <c r="N34" t="n">
+        <v>0.02748308476622072</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35" t="n">
@@ -1773,6 +1981,12 @@
       <c r="L35" t="n">
         <v>0.8825908174455211</v>
       </c>
+      <c r="M35" t="n">
+        <v>0.001601413773720076</v>
+      </c>
+      <c r="N35" t="n">
+        <v>0.009512660995420098</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="n">
@@ -1811,6 +2025,12 @@
       <c r="L36" t="n">
         <v>0.8528993260333869</v>
       </c>
+      <c r="M36" t="n">
+        <v>0.005503741485540608</v>
+      </c>
+      <c r="N36" t="n">
+        <v>0.00275745049986583</v>
+      </c>
     </row>
     <row r="37">
       <c r="A37" t="n">
@@ -1849,6 +2069,12 @@
       <c r="L37" t="n">
         <v>0.7533500533551098</v>
       </c>
+      <c r="M37" t="n">
+        <v>0.001365907260505511</v>
+      </c>
+      <c r="N37" t="n">
+        <v>0.01115611759469526</v>
+      </c>
     </row>
     <row r="38">
       <c r="A38" t="n">
@@ -1887,6 +2113,12 @@
       <c r="L38" t="n">
         <v>0.9430534863174301</v>
       </c>
+      <c r="M38" t="n">
+        <v>0.001604023663187708</v>
+      </c>
+      <c r="N38" t="n">
+        <v>0.009497025664011357</v>
+      </c>
     </row>
     <row r="39">
       <c r="A39" t="n">
@@ -1925,6 +2157,12 @@
       <c r="L39" t="n">
         <v>0.8334106047097524</v>
       </c>
+      <c r="M39" t="n">
+        <v>0.0006902106151281438</v>
+      </c>
+      <c r="N39" t="n">
+        <v>0.022095318298779</v>
+      </c>
     </row>
     <row r="40">
       <c r="A40" t="n">
@@ -1963,6 +2201,12 @@
       <c r="L40" t="n">
         <v>0.8973996384701534</v>
       </c>
+      <c r="M40" t="n">
+        <v>0.002141982431520233</v>
+      </c>
+      <c r="N40" t="n">
+        <v>0.007108568562547757</v>
+      </c>
     </row>
     <row r="41">
       <c r="A41" t="n">
@@ -2001,6 +2245,12 @@
       <c r="L41" t="n">
         <v>0.882247705324954</v>
       </c>
+      <c r="M41" t="n">
+        <v>0.001218390539737519</v>
+      </c>
+      <c r="N41" t="n">
+        <v>0.01250844591799572</v>
+      </c>
     </row>
     <row r="42">
       <c r="A42" t="n">
@@ -2039,6 +2289,12 @@
       <c r="L42" t="n">
         <v>0.8411686235652179</v>
       </c>
+      <c r="M42" t="n">
+        <v>0.001073883397341757</v>
+      </c>
+      <c r="N42" t="n">
+        <v>0.01419386148361095</v>
+      </c>
     </row>
     <row r="43">
       <c r="A43" t="n">
@@ -2077,6 +2333,12 @@
       <c r="L43" t="n">
         <v>0.8411370940962766</v>
       </c>
+      <c r="M43" t="n">
+        <v>0.001602704545825947</v>
+      </c>
+      <c r="N43" t="n">
+        <v>0.009507322582351426</v>
+      </c>
     </row>
     <row r="44">
       <c r="A44" t="n">
@@ -2115,6 +2377,12 @@
       <c r="L44" t="n">
         <v>0.925291187858681</v>
       </c>
+      <c r="M44" t="n">
+        <v>0.001475378567691946</v>
+      </c>
+      <c r="N44" t="n">
+        <v>0.01032885906651404</v>
+      </c>
     </row>
     <row r="45">
       <c r="A45" t="n">
@@ -2153,6 +2421,12 @@
       <c r="L45" t="n">
         <v>0.9369872208320694</v>
       </c>
+      <c r="M45" t="n">
+        <v>0.005284186856818299</v>
+      </c>
+      <c r="N45" t="n">
+        <v>0.002872026527797469</v>
+      </c>
     </row>
     <row r="46">
       <c r="A46" t="n">
@@ -2191,6 +2465,12 @@
       <c r="L46" t="n">
         <v>0.8401804068369867</v>
       </c>
+      <c r="M46" t="n">
+        <v>0.001029526635234823</v>
+      </c>
+      <c r="N46" t="n">
+        <v>0.01480603845920722</v>
+      </c>
     </row>
     <row r="47">
       <c r="A47" t="n">
@@ -2229,6 +2509,12 @@
       <c r="L47" t="n">
         <v>0.9619299457081082</v>
       </c>
+      <c r="M47" t="n">
+        <v>0.006405716922411627</v>
+      </c>
+      <c r="N47" t="n">
+        <v>0.002366423563901385</v>
+      </c>
     </row>
     <row r="48">
       <c r="A48" t="n">
@@ -2267,6 +2553,12 @@
       <c r="L48" t="n">
         <v>0.7074879559819353</v>
       </c>
+      <c r="M48" t="n">
+        <v>0.0007385354315197154</v>
+      </c>
+      <c r="N48" t="n">
+        <v>0.0206457565402557</v>
+      </c>
     </row>
     <row r="49">
       <c r="A49" t="n">
@@ -2305,6 +2597,12 @@
       <c r="L49" t="n">
         <v>0.558086879855652</v>
       </c>
+      <c r="M49" t="n">
+        <v>0.002074629197566057</v>
+      </c>
+      <c r="N49" t="n">
+        <v>0.007339914090364243</v>
+      </c>
     </row>
     <row r="50">
       <c r="A50" t="n">
@@ -2343,6 +2641,12 @@
       <c r="L50" t="n">
         <v>0.8539705548632326</v>
       </c>
+      <c r="M50" t="n">
+        <v>0.001133518762959794</v>
+      </c>
+      <c r="N50" t="n">
+        <v>0.01344582298428955</v>
+      </c>
     </row>
     <row r="51">
       <c r="A51" t="n">
@@ -2381,6 +2685,12 @@
       <c r="L51" t="n">
         <v>0.9643666521702212</v>
       </c>
+      <c r="M51" t="n">
+        <v>0.004581591482460857</v>
+      </c>
+      <c r="N51" t="n">
+        <v>0.003315460112848903</v>
+      </c>
     </row>
     <row r="52">
       <c r="A52" t="n">
@@ -2419,6 +2729,12 @@
       <c r="L52" t="n">
         <v>0.7513386038279505</v>
       </c>
+      <c r="M52" t="n">
+        <v>0.0005941609203614671</v>
+      </c>
+      <c r="N52" t="n">
+        <v>0.02566618648415696</v>
+      </c>
     </row>
     <row r="53">
       <c r="A53" t="n">
@@ -2457,6 +2773,12 @@
       <c r="L53" t="n">
         <v>0.9111022300455747</v>
       </c>
+      <c r="M53" t="n">
+        <v>0.00602188472710978</v>
+      </c>
+      <c r="N53" t="n">
+        <v>0.002518800326011809</v>
+      </c>
     </row>
     <row r="54">
       <c r="A54" t="n">
@@ -2495,6 +2817,12 @@
       <c r="L54" t="n">
         <v>0.9278138691864173</v>
       </c>
+      <c r="M54" t="n">
+        <v>0.002191718429965062</v>
+      </c>
+      <c r="N54" t="n">
+        <v>0.00694419428264677</v>
+      </c>
     </row>
     <row r="55">
       <c r="A55" t="n">
@@ -2533,6 +2861,12 @@
       <c r="L55" t="n">
         <v>0.9059768476092575</v>
       </c>
+      <c r="M55" t="n">
+        <v>0.00142195508856449</v>
+      </c>
+      <c r="N55" t="n">
+        <v>0.01071562543997999</v>
+      </c>
     </row>
     <row r="56">
       <c r="A56" t="n">
@@ -2571,6 +2905,12 @@
       <c r="L56" t="n">
         <v>0.9041802821117215</v>
       </c>
+      <c r="M56" t="n">
+        <v>0.001379334672824501</v>
+      </c>
+      <c r="N56" t="n">
+        <v>0.01104700359070773</v>
+      </c>
     </row>
     <row r="57">
       <c r="A57" t="n">
@@ -2609,6 +2949,12 @@
       <c r="L57" t="n">
         <v>0.9030450645367402</v>
       </c>
+      <c r="M57" t="n">
+        <v>0.00147921018470051</v>
+      </c>
+      <c r="N57" t="n">
+        <v>0.01030040538680741</v>
+      </c>
     </row>
     <row r="58">
       <c r="A58" t="n">
@@ -2647,6 +2993,12 @@
       <c r="L58" t="n">
         <v>0.9810063516136202</v>
       </c>
+      <c r="M58" t="n">
+        <v>0.02007928639559011</v>
+      </c>
+      <c r="N58" t="n">
+        <v>0.000744502262478377</v>
+      </c>
     </row>
     <row r="59">
       <c r="A59" t="n">
@@ -2685,6 +3037,12 @@
       <c r="L59" t="n">
         <v>0.9872626376361471</v>
       </c>
+      <c r="M59" t="n">
+        <v>0.01864416531466991</v>
+      </c>
+      <c r="N59" t="n">
+        <v>0.0008036048126524054</v>
+      </c>
     </row>
     <row r="60">
       <c r="A60" t="n">
@@ -2723,6 +3081,12 @@
       <c r="L60" t="n">
         <v>0.7308721169317417</v>
       </c>
+      <c r="M60" t="n">
+        <v>0.0007047313122505532</v>
+      </c>
+      <c r="N60" t="n">
+        <v>0.02163613326251378</v>
+      </c>
     </row>
     <row r="61">
       <c r="A61" t="n">
@@ -2761,6 +3125,12 @@
       <c r="L61" t="n">
         <v>0.9278188610814054</v>
       </c>
+      <c r="M61" t="n">
+        <v>0.003141059721334884</v>
+      </c>
+      <c r="N61" t="n">
+        <v>0.004842560121306905</v>
+      </c>
     </row>
     <row r="62">
       <c r="A62" t="n">
@@ -2799,6 +3169,12 @@
       <c r="L62" t="n">
         <v>0.9836755177012017</v>
       </c>
+      <c r="M62" t="n">
+        <v>0.02607928515951173</v>
+      </c>
+      <c r="N62" t="n">
+        <v>0.0005702332777043848</v>
+      </c>
     </row>
     <row r="63">
       <c r="A63" t="n">
@@ -2837,6 +3213,12 @@
       <c r="L63" t="n">
         <v>0.9198364492038837</v>
       </c>
+      <c r="M63" t="n">
+        <v>0.003108699381834375</v>
+      </c>
+      <c r="N63" t="n">
+        <v>0.004892951160001898</v>
+      </c>
     </row>
     <row r="64">
       <c r="A64" t="n">
@@ -2875,6 +3257,12 @@
       <c r="L64" t="n">
         <v>0.8091440238916799</v>
       </c>
+      <c r="M64" t="n">
+        <v>0.001178952913507219</v>
+      </c>
+      <c r="N64" t="n">
+        <v>0.01292751796629175</v>
+      </c>
     </row>
     <row r="65">
       <c r="A65" t="n">
@@ -2913,6 +3301,12 @@
       <c r="L65" t="n">
         <v>0.8257490242133041</v>
       </c>
+      <c r="M65" t="n">
+        <v>0.0008734620513135534</v>
+      </c>
+      <c r="N65" t="n">
+        <v>0.01745393035501193</v>
+      </c>
     </row>
     <row r="66">
       <c r="A66" t="n">
@@ -2951,6 +3345,12 @@
       <c r="L66" t="n">
         <v>0.9921347894076566</v>
       </c>
+      <c r="M66" t="n">
+        <v>0.03356292133424394</v>
+      </c>
+      <c r="N66" t="n">
+        <v>0.0004385213440148785</v>
+      </c>
     </row>
     <row r="67">
       <c r="A67" t="n">
@@ -2989,6 +3389,12 @@
       <c r="L67" t="n">
         <v>0.8295218560042373</v>
       </c>
+      <c r="M67" t="n">
+        <v>0.0008662768990181331</v>
+      </c>
+      <c r="N67" t="n">
+        <v>0.0175991346919927</v>
+      </c>
     </row>
     <row r="68">
       <c r="A68" t="n">
@@ -3027,6 +3433,12 @@
       <c r="L68" t="n">
         <v>0.7728536612176758</v>
       </c>
+      <c r="M68" t="n">
+        <v>0.0009454571852267627</v>
+      </c>
+      <c r="N68" t="n">
+        <v>0.01612393491768974</v>
+      </c>
     </row>
     <row r="69">
       <c r="A69" t="n">
@@ -3065,6 +3477,12 @@
       <c r="L69" t="n">
         <v>0.9095302348460937</v>
       </c>
+      <c r="M69" t="n">
+        <v>0.002446127177154327</v>
+      </c>
+      <c r="N69" t="n">
+        <v>0.006222327906593267</v>
+      </c>
     </row>
     <row r="70">
       <c r="A70" t="n">
@@ -3103,6 +3521,12 @@
       <c r="L70" t="n">
         <v>0.9398685045249683</v>
       </c>
+      <c r="M70" t="n">
+        <v>0.005198616023328618</v>
+      </c>
+      <c r="N70" t="n">
+        <v>0.00291988365222893</v>
+      </c>
     </row>
     <row r="71">
       <c r="A71" t="n">
@@ -3141,6 +3565,12 @@
       <c r="L71" t="n">
         <v>0.891683179792828</v>
       </c>
+      <c r="M71" t="n">
+        <v>0.002323259623694773</v>
+      </c>
+      <c r="N71" t="n">
+        <v>0.00655275800425068</v>
+      </c>
     </row>
     <row r="72">
       <c r="A72" t="n">
@@ -3179,6 +3609,12 @@
       <c r="L72" t="n">
         <v>0.8022367164683548</v>
       </c>
+      <c r="M72" t="n">
+        <v>0.0009504928712252124</v>
+      </c>
+      <c r="N72" t="n">
+        <v>0.01604000418879857</v>
+      </c>
     </row>
     <row r="73">
       <c r="A73" t="n">
@@ -3217,6 +3653,12 @@
       <c r="L73" t="n">
         <v>0.9970020100760538</v>
       </c>
+      <c r="M73" t="n">
+        <v>0.04993690310693354</v>
+      </c>
+      <c r="N73" t="n">
+        <v>0.0002905641288075114</v>
+      </c>
     </row>
     <row r="74">
       <c r="A74" t="n">
@@ -3255,6 +3697,12 @@
       <c r="L74" t="n">
         <v>0.9008841269086348</v>
       </c>
+      <c r="M74" t="n">
+        <v>0.0008842160865769275</v>
+      </c>
+      <c r="N74" t="n">
+        <v>0.01724663890270542</v>
+      </c>
     </row>
     <row r="75">
       <c r="A75" t="n">
@@ -3293,6 +3741,12 @@
       <c r="L75" t="n">
         <v>0.9851049822036493</v>
       </c>
+      <c r="M75" t="n">
+        <v>0.02972948130286961</v>
+      </c>
+      <c r="N75" t="n">
+        <v>0.0004983603318359005</v>
+      </c>
     </row>
     <row r="76">
       <c r="A76" t="n">
@@ -3331,6 +3785,12 @@
       <c r="L76" t="n">
         <v>0.8718104495061474</v>
       </c>
+      <c r="M76" t="n">
+        <v>0.001026845807331529</v>
+      </c>
+      <c r="N76" t="n">
+        <v>0.01484650809515478</v>
+      </c>
     </row>
     <row r="77">
       <c r="A77" t="n">
@@ -3369,6 +3829,12 @@
       <c r="L77" t="n">
         <v>0.9930629616868386</v>
       </c>
+      <c r="M77" t="n">
+        <v>0.04812438912496883</v>
+      </c>
+      <c r="N77" t="n">
+        <v>0.0003026092124609467</v>
+      </c>
     </row>
     <row r="78">
       <c r="A78" t="n">
@@ -3407,6 +3873,12 @@
       <c r="L78" t="n">
         <v>0.9929381805900399</v>
       </c>
+      <c r="M78" t="n">
+        <v>0.02614375540538424</v>
+      </c>
+      <c r="N78" t="n">
+        <v>0.0005690710992158112</v>
+      </c>
     </row>
     <row r="79">
       <c r="A79" t="n">
@@ -3445,6 +3917,12 @@
       <c r="L79" t="n">
         <v>0.822232776339952</v>
       </c>
+      <c r="M79" t="n">
+        <v>0.0005792260291903144</v>
+      </c>
+      <c r="N79" t="n">
+        <v>0.02632889600747445</v>
+      </c>
     </row>
     <row r="80">
       <c r="A80" t="n">
@@ -3483,6 +3961,12 @@
       <c r="L80" t="n">
         <v>0.9647802390873376</v>
       </c>
+      <c r="M80" t="n">
+        <v>0.005608185232517342</v>
+      </c>
+      <c r="N80" t="n">
+        <v>0.002705421865395328</v>
+      </c>
     </row>
     <row r="81">
       <c r="A81" t="n">
@@ -3521,6 +4005,12 @@
       <c r="L81" t="n">
         <v>0.9192016006386268</v>
       </c>
+      <c r="M81" t="n">
+        <v>0.001523305313841515</v>
+      </c>
+      <c r="N81" t="n">
+        <v>0.01000166324937988</v>
+      </c>
     </row>
     <row r="82">
       <c r="A82" t="n">
@@ -3559,6 +4049,12 @@
       <c r="L82" t="n">
         <v>0.8845452214757624</v>
       </c>
+      <c r="M82" t="n">
+        <v>0.01017572157137595</v>
+      </c>
+      <c r="N82" t="n">
+        <v>0.001484604084868556</v>
+      </c>
     </row>
     <row r="83">
       <c r="A83" t="n">
@@ -3597,6 +4093,12 @@
       <c r="L83" t="n">
         <v>0.8859869366000226</v>
       </c>
+      <c r="M83" t="n">
+        <v>0.0014042327430546</v>
+      </c>
+      <c r="N83" t="n">
+        <v>0.01084991513720296</v>
+      </c>
     </row>
     <row r="84">
       <c r="A84" t="n">
@@ -3635,6 +4137,12 @@
       <c r="L84" t="n">
         <v>0.9785921765618859</v>
       </c>
+      <c r="M84" t="n">
+        <v>0.009628284330985686</v>
+      </c>
+      <c r="N84" t="n">
+        <v>0.001569607113267809</v>
+      </c>
     </row>
     <row r="85">
       <c r="A85" t="n">
@@ -3673,6 +4181,12 @@
       <c r="L85" t="n">
         <v>0.9928073213053636</v>
       </c>
+      <c r="M85" t="n">
+        <v>0.03870860721629107</v>
+      </c>
+      <c r="N85" t="n">
+        <v>0.0003792465906676159</v>
+      </c>
     </row>
     <row r="86">
       <c r="A86" t="n">
@@ -3711,6 +4225,12 @@
       <c r="L86" t="n">
         <v>0.9759002959708966</v>
       </c>
+      <c r="M86" t="n">
+        <v>0.01553319608427437</v>
+      </c>
+      <c r="N86" t="n">
+        <v>0.0009666586271102258</v>
+      </c>
     </row>
     <row r="87">
       <c r="A87" t="n">
@@ -3749,6 +4269,12 @@
       <c r="L87" t="n">
         <v>0.6879158826621802</v>
       </c>
+      <c r="M87" t="n">
+        <v>0.001703239810145779</v>
+      </c>
+      <c r="N87" t="n">
+        <v>0.008943623186578572</v>
+      </c>
     </row>
     <row r="88">
       <c r="A88" t="n">
@@ -3787,6 +4313,12 @@
       <c r="L88" t="n">
         <v>0.6535873365655547</v>
       </c>
+      <c r="M88" t="n">
+        <v>0.00186402780789889</v>
+      </c>
+      <c r="N88" t="n">
+        <v>0.008170738728088212</v>
+      </c>
     </row>
     <row r="89">
       <c r="A89" t="n">
@@ -3825,6 +4357,12 @@
       <c r="L89" t="n">
         <v>0.9073554011900521</v>
       </c>
+      <c r="M89" t="n">
+        <v>0.002840640001827659</v>
+      </c>
+      <c r="N89" t="n">
+        <v>0.005356531032328506</v>
+      </c>
     </row>
     <row r="90">
       <c r="A90" t="n">
@@ -3863,6 +4401,12 @@
       <c r="L90" t="n">
         <v>0.9915434731372118</v>
       </c>
+      <c r="M90" t="n">
+        <v>0.03568552181140604</v>
+      </c>
+      <c r="N90" t="n">
+        <v>0.0004128482280695085</v>
+      </c>
     </row>
     <row r="91">
       <c r="A91" t="n">
@@ -3901,6 +4445,12 @@
       <c r="L91" t="n">
         <v>0.9684737768977113</v>
       </c>
+      <c r="M91" t="n">
+        <v>0.008029159341380966</v>
+      </c>
+      <c r="N91" t="n">
+        <v>0.001885424500205245</v>
+      </c>
     </row>
     <row r="92">
       <c r="A92" t="n">
@@ -3939,6 +4489,12 @@
       <c r="L92" t="n">
         <v>0.9961336048776153</v>
       </c>
+      <c r="M92" t="n">
+        <v>0.05534404994255956</v>
+      </c>
+      <c r="N92" t="n">
+        <v>0.0002605840738508986</v>
+      </c>
     </row>
     <row r="93">
       <c r="A93" t="n">
@@ -3977,6 +4533,12 @@
       <c r="L93" t="n">
         <v>0.9807775664623751</v>
       </c>
+      <c r="M93" t="n">
+        <v>0.007362693969224779</v>
+      </c>
+      <c r="N93" t="n">
+        <v>0.002056886571979022</v>
+      </c>
     </row>
     <row r="94">
       <c r="A94" t="n">
@@ -4015,6 +4577,12 @@
       <c r="L94" t="n">
         <v>0.8946012928100033</v>
       </c>
+      <c r="M94" t="n">
+        <v>0.001764019038030116</v>
+      </c>
+      <c r="N94" t="n">
+        <v>0.008634259672040569</v>
+      </c>
     </row>
     <row r="95">
       <c r="A95" t="n">
@@ -4053,6 +4621,12 @@
       <c r="L95" t="n">
         <v>0.9938427576975253</v>
       </c>
+      <c r="M95" t="n">
+        <v>0.03119790910756507</v>
+      </c>
+      <c r="N95" t="n">
+        <v>0.0004733098957863783</v>
+      </c>
     </row>
     <row r="96">
       <c r="A96" t="n">
@@ -4091,6 +4665,12 @@
       <c r="L96" t="n">
         <v>0.9410521381536906</v>
       </c>
+      <c r="M96" t="n">
+        <v>0.002061039494605826</v>
+      </c>
+      <c r="N96" t="n">
+        <v>0.007387077666554844</v>
+      </c>
     </row>
     <row r="97">
       <c r="A97" t="n">
@@ -4129,6 +4709,12 @@
       <c r="L97" t="n">
         <v>0.8678819366682063</v>
       </c>
+      <c r="M97" t="n">
+        <v>0.001897743502249361</v>
+      </c>
+      <c r="N97" t="n">
+        <v>0.008027105283970354</v>
+      </c>
     </row>
     <row r="98">
       <c r="A98" t="n">
@@ -4167,6 +4753,12 @@
       <c r="L98" t="n">
         <v>0.9399562184629752</v>
       </c>
+      <c r="M98" t="n">
+        <v>0.003778875606600898</v>
+      </c>
+      <c r="N98" t="n">
+        <v>0.004022844317080922</v>
+      </c>
     </row>
     <row r="99">
       <c r="A99" t="n">
@@ -4205,6 +4797,12 @@
       <c r="L99" t="n">
         <v>0.9008253122154286</v>
       </c>
+      <c r="M99" t="n">
+        <v>0.001369736361388359</v>
+      </c>
+      <c r="N99" t="n">
+        <v>0.01112442442453017</v>
+      </c>
     </row>
     <row r="100">
       <c r="A100" t="n">
@@ -4243,6 +4841,12 @@
       <c r="L100" t="n">
         <v>0.5829456681189431</v>
       </c>
+      <c r="M100" t="n">
+        <v>0.0005327667763778629</v>
+      </c>
+      <c r="N100" t="n">
+        <v>0.02862552264162835</v>
+      </c>
     </row>
     <row r="101">
       <c r="A101" t="n">
@@ -4281,6 +4885,12 @@
       <c r="L101" t="n">
         <v>0.8869701271015727</v>
       </c>
+      <c r="M101" t="n">
+        <v>0.00168460273043604</v>
+      </c>
+      <c r="N101" t="n">
+        <v>0.009042573153903879</v>
+      </c>
     </row>
     <row r="102">
       <c r="A102" t="n">
@@ -4319,6 +4929,12 @@
       <c r="L102" t="n">
         <v>0.9080673329686686</v>
       </c>
+      <c r="M102" t="n">
+        <v>0.004663907653826278</v>
+      </c>
+      <c r="N102" t="n">
+        <v>0.003256113342693744</v>
+      </c>
     </row>
     <row r="103">
       <c r="A103" t="n">
@@ -4357,6 +4973,12 @@
       <c r="L103" t="n">
         <v>0.8969471340712724</v>
       </c>
+      <c r="M103" t="n">
+        <v>0.001111474282707306</v>
+      </c>
+      <c r="N103" t="n">
+        <v>0.01371495536036191</v>
+      </c>
     </row>
     <row r="104">
       <c r="A104" t="n">
@@ -4395,6 +5017,12 @@
       <c r="L104" t="n">
         <v>0.9340678455406179</v>
       </c>
+      <c r="M104" t="n">
+        <v>0.003961029333702738</v>
+      </c>
+      <c r="N104" t="n">
+        <v>0.003837167701036918</v>
+      </c>
     </row>
     <row r="105">
       <c r="A105" t="n">
@@ -4433,6 +5061,12 @@
       <c r="L105" t="n">
         <v>0.8650669706647534</v>
       </c>
+      <c r="M105" t="n">
+        <v>0.001184782640116442</v>
+      </c>
+      <c r="N105" t="n">
+        <v>0.01286546256736935</v>
+      </c>
     </row>
     <row r="106">
       <c r="A106" t="n">
@@ -4471,6 +5105,12 @@
       <c r="L106" t="n">
         <v>0.9772696547372196</v>
       </c>
+      <c r="M106" t="n">
+        <v>0.007553980255894144</v>
+      </c>
+      <c r="N106" t="n">
+        <v>0.002004512868207901</v>
+      </c>
     </row>
     <row r="107">
       <c r="A107" t="n">
@@ -4509,6 +5149,12 @@
       <c r="L107" t="n">
         <v>0.9243805073109801</v>
       </c>
+      <c r="M107" t="n">
+        <v>0.001702053983143623</v>
+      </c>
+      <c r="N107" t="n">
+        <v>0.008949651320417288</v>
+      </c>
     </row>
     <row r="108">
       <c r="A108" t="n">
@@ -4547,6 +5193,12 @@
       <c r="L108" t="n">
         <v>0.7795163810530594</v>
       </c>
+      <c r="M108" t="n">
+        <v>0.003467710787853873</v>
+      </c>
+      <c r="N108" t="n">
+        <v>0.004385197507797588</v>
+      </c>
     </row>
     <row r="109">
       <c r="A109" t="n">
@@ -4585,6 +5237,12 @@
       <c r="L109" t="n">
         <v>0.9601385332144944</v>
       </c>
+      <c r="M109" t="n">
+        <v>0.003848891833719489</v>
+      </c>
+      <c r="N109" t="n">
+        <v>0.003947019651356722</v>
+      </c>
     </row>
     <row r="110">
       <c r="A110" t="n">
@@ -4623,6 +5281,12 @@
       <c r="L110" t="n">
         <v>0.9549697285318902</v>
       </c>
+      <c r="M110" t="n">
+        <v>0.002311377440491292</v>
+      </c>
+      <c r="N110" t="n">
+        <v>0.006585378368191424</v>
+      </c>
     </row>
     <row r="111">
       <c r="A111" t="n">
@@ -4661,6 +5325,12 @@
       <c r="L111" t="n">
         <v>0.5103474671154898</v>
       </c>
+      <c r="M111" t="n">
+        <v>0.00169869456312271</v>
+      </c>
+      <c r="N111" t="n">
+        <v>0.008967603180455083</v>
+      </c>
     </row>
     <row r="112">
       <c r="A112" t="n">
@@ -4699,6 +5369,12 @@
       <c r="L112" t="n">
         <v>0.9484988069603483</v>
       </c>
+      <c r="M112" t="n">
+        <v>0.003486592307374266</v>
+      </c>
+      <c r="N112" t="n">
+        <v>0.004361253957740707</v>
+      </c>
     </row>
     <row r="113">
       <c r="A113" t="n">
@@ -4737,6 +5413,12 @@
       <c r="L113" t="n">
         <v>0.960058046908946</v>
       </c>
+      <c r="M113" t="n">
+        <v>0.002553849544576573</v>
+      </c>
+      <c r="N113" t="n">
+        <v>0.005958253517743345</v>
+      </c>
     </row>
     <row r="114">
       <c r="A114" t="n">
@@ -4775,6 +5457,12 @@
       <c r="L114" t="n">
         <v>0.855270116968601</v>
       </c>
+      <c r="M114" t="n">
+        <v>0.001769912896360867</v>
+      </c>
+      <c r="N114" t="n">
+        <v>0.008606033237537843</v>
+      </c>
     </row>
     <row r="115">
       <c r="A115" t="n">
@@ -4813,6 +5501,12 @@
       <c r="L115" t="n">
         <v>0.8808877340095371</v>
       </c>
+      <c r="M115" t="n">
+        <v>0.00184277478739219</v>
+      </c>
+      <c r="N115" t="n">
+        <v>0.008265059751092169</v>
+      </c>
     </row>
     <row r="116">
       <c r="A116" t="n">
@@ -4851,6 +5545,12 @@
       <c r="L116" t="n">
         <v>0.9321757998343589</v>
       </c>
+      <c r="M116" t="n">
+        <v>0.002346786591239714</v>
+      </c>
+      <c r="N116" t="n">
+        <v>0.006486912425743506</v>
+      </c>
     </row>
     <row r="117">
       <c r="A117" t="n">
@@ -4889,6 +5589,12 @@
       <c r="L117" t="n">
         <v>0.9949097860756955</v>
       </c>
+      <c r="M117" t="n">
+        <v>0.0638329795316893</v>
+      </c>
+      <c r="N117" t="n">
+        <v>0.0002241671061152589</v>
+      </c>
     </row>
     <row r="118">
       <c r="A118" t="n">
@@ -4927,6 +5633,12 @@
       <c r="L118" t="n">
         <v>0.8922552142478214</v>
       </c>
+      <c r="M118" t="n">
+        <v>0.0009581685962968431</v>
+      </c>
+      <c r="N118" t="n">
+        <v>0.01591227681277931</v>
+      </c>
     </row>
     <row r="119">
       <c r="A119" t="n">
@@ -4965,6 +5677,12 @@
       <c r="L119" t="n">
         <v>0.9872513737986526</v>
       </c>
+      <c r="M119" t="n">
+        <v>0.02844394678351496</v>
+      </c>
+      <c r="N119" t="n">
+        <v>0.0005215588224473846</v>
+      </c>
     </row>
     <row r="120">
       <c r="A120" t="n">
@@ -5003,6 +5721,12 @@
       <c r="L120" t="n">
         <v>0.9141391443627839</v>
       </c>
+      <c r="M120" t="n">
+        <v>0.001791883715532152</v>
+      </c>
+      <c r="N120" t="n">
+        <v>0.008500367614255501</v>
+      </c>
     </row>
     <row r="121">
       <c r="A121" t="n">
@@ -5041,6 +5765,12 @@
       <c r="L121" t="n">
         <v>0.9387210274159511</v>
       </c>
+      <c r="M121" t="n">
+        <v>0.001923632551071183</v>
+      </c>
+      <c r="N121" t="n">
+        <v>0.007917024572274259</v>
+      </c>
     </row>
     <row r="122">
       <c r="A122" t="n">
@@ -5079,6 +5809,12 @@
       <c r="L122" t="n">
         <v>0.955463478573761</v>
       </c>
+      <c r="M122" t="n">
+        <v>0.004846410811011308</v>
+      </c>
+      <c r="N122" t="n">
+        <v>0.00313291979186317</v>
+      </c>
     </row>
     <row r="123">
       <c r="A123" t="n">
@@ -5117,6 +5853,12 @@
       <c r="L123" t="n">
         <v>0.9086613423653298</v>
       </c>
+      <c r="M123" t="n">
+        <v>0.005674646564179374</v>
+      </c>
+      <c r="N123" t="n">
+        <v>0.002673798577769765</v>
+      </c>
     </row>
     <row r="124">
       <c r="A124" t="n">
@@ -5155,6 +5897,12 @@
       <c r="L124" t="n">
         <v>0.8442314299313889</v>
       </c>
+      <c r="M124" t="n">
+        <v>0.001068630531673853</v>
+      </c>
+      <c r="N124" t="n">
+        <v>0.01426367731000806</v>
+      </c>
     </row>
     <row r="125">
       <c r="A125" t="n">
@@ -5193,6 +5941,12 @@
       <c r="L125" t="n">
         <v>0.8203891455913085</v>
       </c>
+      <c r="M125" t="n">
+        <v>0.0009272395796195385</v>
+      </c>
+      <c r="N125" t="n">
+        <v>0.01644042194997824</v>
+      </c>
     </row>
     <row r="126">
       <c r="A126" t="n">
@@ -5231,6 +5985,12 @@
       <c r="L126" t="n">
         <v>0.9226450119070091</v>
       </c>
+      <c r="M126" t="n">
+        <v>0.001213859615906759</v>
+      </c>
+      <c r="N126" t="n">
+        <v>0.01256286503585619</v>
+      </c>
     </row>
     <row r="127">
       <c r="A127" t="n">
@@ -5269,6 +6029,12 @@
       <c r="L127" t="n">
         <v>0.8761147354758003</v>
       </c>
+      <c r="M127" t="n">
+        <v>0.001261165988811307</v>
+      </c>
+      <c r="N127" t="n">
+        <v>0.01208355856290956</v>
+      </c>
     </row>
     <row r="128">
       <c r="A128" t="n">
@@ -5307,6 +6073,12 @@
       <c r="L128" t="n">
         <v>0.897102218971887</v>
       </c>
+      <c r="M128" t="n">
+        <v>0.001402893657949393</v>
+      </c>
+      <c r="N128" t="n">
+        <v>0.01086130256435531</v>
+      </c>
     </row>
     <row r="129">
       <c r="A129" t="n">
@@ -5345,6 +6117,12 @@
       <c r="L129" t="n">
         <v>0.9428971175280685</v>
       </c>
+      <c r="M129" t="n">
+        <v>0.001843990103132003</v>
+      </c>
+      <c r="N129" t="n">
+        <v>0.00825735368536014</v>
+      </c>
     </row>
     <row r="130">
       <c r="A130" t="n">
@@ -5383,6 +6161,12 @@
       <c r="L130" t="n">
         <v>0.9287545451556243</v>
       </c>
+      <c r="M130" t="n">
+        <v>0.002054778098600284</v>
+      </c>
+      <c r="N130" t="n">
+        <v>0.007410211811921359</v>
+      </c>
     </row>
     <row r="131">
       <c r="A131" t="n">
@@ -5421,6 +6205,12 @@
       <c r="L131" t="n">
         <v>0.8565662408598148</v>
       </c>
+      <c r="M131" t="n">
+        <v>0.002082175872670076</v>
+      </c>
+      <c r="N131" t="n">
+        <v>0.007313186724547415</v>
+      </c>
     </row>
     <row r="132">
       <c r="A132" t="n">
@@ -5459,6 +6249,12 @@
       <c r="L132" t="n">
         <v>0.8392187630858511</v>
       </c>
+      <c r="M132" t="n">
+        <v>0.0009746419927825702</v>
+      </c>
+      <c r="N132" t="n">
+        <v>0.01564034775935002</v>
+      </c>
     </row>
     <row r="133">
       <c r="A133" t="n">
@@ -5497,6 +6293,12 @@
       <c r="L133" t="n">
         <v>0.9346334661754314</v>
       </c>
+      <c r="M133" t="n">
+        <v>0.003411727612716884</v>
+      </c>
+      <c r="N133" t="n">
+        <v>0.004456964759575042</v>
+      </c>
     </row>
     <row r="134">
       <c r="A134" t="n">
@@ -5535,6 +6337,12 @@
       <c r="L134" t="n">
         <v>0.9430161630514329</v>
       </c>
+      <c r="M134" t="n">
+        <v>0.001846339646084996</v>
+      </c>
+      <c r="N134" t="n">
+        <v>0.008246833793944273</v>
+      </c>
     </row>
     <row r="135">
       <c r="A135" t="n">
@@ -5573,6 +6381,12 @@
       <c r="L135" t="n">
         <v>0.98731805300122</v>
       </c>
+      <c r="M135" t="n">
+        <v>0.04029102289864368</v>
+      </c>
+      <c r="N135" t="n">
+        <v>0.0003639272624151964</v>
+      </c>
     </row>
     <row r="136">
       <c r="A136" t="n">
@@ -5611,6 +6425,12 @@
       <c r="L136" t="n">
         <v>0.9179759187452697</v>
       </c>
+      <c r="M136" t="n">
+        <v>0.002010419992671556</v>
+      </c>
+      <c r="N136" t="n">
+        <v>0.007574452902861756</v>
+      </c>
     </row>
     <row r="137">
       <c r="A137" t="n">
@@ -5649,6 +6469,12 @@
       <c r="L137" t="n">
         <v>0.8986123184511344</v>
       </c>
+      <c r="M137" t="n">
+        <v>0.002426914099612207</v>
+      </c>
+      <c r="N137" t="n">
+        <v>0.00627223065773921</v>
+      </c>
     </row>
     <row r="138">
       <c r="A138" t="n">
@@ -5687,6 +6513,12 @@
       <c r="L138" t="n">
         <v>0.8336192812375283</v>
       </c>
+      <c r="M138" t="n">
+        <v>0.001159825638912387</v>
+      </c>
+      <c r="N138" t="n">
+        <v>0.01314028462186679</v>
+      </c>
     </row>
     <row r="139">
       <c r="A139" t="n">
@@ -5725,6 +6557,12 @@
       <c r="L139" t="n">
         <v>0.8263924217819224</v>
       </c>
+      <c r="M139" t="n">
+        <v>0.001236823582631623</v>
+      </c>
+      <c r="N139" t="n">
+        <v>0.01232192310653928</v>
+      </c>
     </row>
     <row r="140">
       <c r="A140" t="n">
@@ -5763,6 +6601,12 @@
       <c r="L140" t="n">
         <v>0.8173567819141898</v>
       </c>
+      <c r="M140" t="n">
+        <v>0.0009006965993840609</v>
+      </c>
+      <c r="N140" t="n">
+        <v>0.01692595729142104</v>
+      </c>
     </row>
     <row r="141">
       <c r="A141" t="n">
@@ -5801,6 +6645,12 @@
       <c r="L141" t="n">
         <v>0.9000440591255729</v>
       </c>
+      <c r="M141" t="n">
+        <v>0.001681771288915922</v>
+      </c>
+      <c r="N141" t="n">
+        <v>0.009057489371769379</v>
+      </c>
     </row>
     <row r="142">
       <c r="A142" t="n">
@@ -5839,6 +6689,12 @@
       <c r="L142" t="n">
         <v>0.8389922205892895</v>
       </c>
+      <c r="M142" t="n">
+        <v>0.001091004236269864</v>
+      </c>
+      <c r="N142" t="n">
+        <v>0.01397071661923893</v>
+      </c>
     </row>
     <row r="143">
       <c r="A143" t="n">
@@ -5877,6 +6733,12 @@
       <c r="L143" t="n">
         <v>0.8946738875047052</v>
       </c>
+      <c r="M143" t="n">
+        <v>0.00176530905457961</v>
+      </c>
+      <c r="N143" t="n">
+        <v>0.008627938777322907</v>
+      </c>
     </row>
     <row r="144">
       <c r="A144" t="n">
@@ -5915,6 +6777,12 @@
       <c r="L144" t="n">
         <v>0.9044548058007221</v>
       </c>
+      <c r="M144" t="n">
+        <v>0.001837426617547739</v>
+      </c>
+      <c r="N144" t="n">
+        <v>0.008289309951091119</v>
+      </c>
     </row>
     <row r="145">
       <c r="A145" t="n">
@@ -5953,6 +6821,12 @@
       <c r="L145" t="n">
         <v>0.7526399157889168</v>
       </c>
+      <c r="M145" t="n">
+        <v>0.001098480083423557</v>
+      </c>
+      <c r="N145" t="n">
+        <v>0.01387563114499216</v>
+      </c>
     </row>
     <row r="146">
       <c r="A146" t="n">
@@ -5991,6 +6865,12 @@
       <c r="L146" t="n">
         <v>0.9262493388689557</v>
       </c>
+      <c r="M146" t="n">
+        <v>0.001978295341288074</v>
+      </c>
+      <c r="N146" t="n">
+        <v>0.007697107571849269</v>
+      </c>
     </row>
     <row r="147">
       <c r="A147" t="n">
@@ -6029,6 +6909,12 @@
       <c r="L147" t="n">
         <v>0.9433236505571059</v>
       </c>
+      <c r="M147" t="n">
+        <v>0.001934589090371758</v>
+      </c>
+      <c r="N147" t="n">
+        <v>0.007869513390420356</v>
+      </c>
     </row>
     <row r="148">
       <c r="A148" t="n">
@@ -6067,6 +6953,12 @@
       <c r="L148" t="n">
         <v>0.9609845841967957</v>
       </c>
+      <c r="M148" t="n">
+        <v>0.01187274069710071</v>
+      </c>
+      <c r="N148" t="n">
+        <v>0.001270264151954779</v>
+      </c>
     </row>
     <row r="149">
       <c r="A149" t="n">
@@ -6105,6 +6997,12 @@
       <c r="L149" t="n">
         <v>0.6100578454053667</v>
       </c>
+      <c r="M149" t="n">
+        <v>0.002686889123878035</v>
+      </c>
+      <c r="N149" t="n">
+        <v>0.005663969236086254</v>
+      </c>
     </row>
     <row r="150">
       <c r="A150" t="n">
@@ -6143,6 +7041,12 @@
       <c r="L150" t="n">
         <v>0.9494487521034845</v>
       </c>
+      <c r="M150" t="n">
+        <v>0.00297874160826142</v>
+      </c>
+      <c r="N150" t="n">
+        <v>0.005103208869262407</v>
+      </c>
     </row>
     <row r="151">
       <c r="A151" t="n">
@@ -6181,6 +7085,12 @@
       <c r="L151" t="n">
         <v>0.9916115253797771</v>
       </c>
+      <c r="M151" t="n">
+        <v>0.0222291791219945</v>
+      </c>
+      <c r="N151" t="n">
+        <v>0.0006710122309564994</v>
+      </c>
     </row>
     <row r="152">
       <c r="A152" t="n">
@@ -6219,6 +7129,12 @@
       <c r="L152" t="n">
         <v>0.973305638315098</v>
       </c>
+      <c r="M152" t="n">
+        <v>0.004018954962533135</v>
+      </c>
+      <c r="N152" t="n">
+        <v>0.003780647551136715</v>
+      </c>
     </row>
     <row r="153">
       <c r="A153" t="n">
@@ -6257,6 +7173,12 @@
       <c r="L153" t="n">
         <v>0.9251518409415673</v>
       </c>
+      <c r="M153" t="n">
+        <v>0.002357280312959839</v>
+      </c>
+      <c r="N153" t="n">
+        <v>0.006457982793384471</v>
+      </c>
     </row>
     <row r="154">
       <c r="A154" t="n">
@@ -6295,6 +7217,12 @@
       <c r="L154" t="n">
         <v>0.8908314478976173</v>
       </c>
+      <c r="M154" t="n">
+        <v>0.002234522002482713</v>
+      </c>
+      <c r="N154" t="n">
+        <v>0.006813236643477518</v>
+      </c>
     </row>
     <row r="155">
       <c r="A155" t="n">
@@ -6333,6 +7261,12 @@
       <c r="L155" t="n">
         <v>0.9625737380906048</v>
       </c>
+      <c r="M155" t="n">
+        <v>0.01021506329683096</v>
+      </c>
+      <c r="N155" t="n">
+        <v>0.001478814925337465</v>
+      </c>
     </row>
     <row r="156">
       <c r="A156" t="n">
@@ -6371,6 +7305,12 @@
       <c r="L156" t="n">
         <v>0.9372808021959397</v>
       </c>
+      <c r="M156" t="n">
+        <v>0.001488685691282324</v>
+      </c>
+      <c r="N156" t="n">
+        <v>0.01023405763790762</v>
+      </c>
     </row>
     <row r="157">
       <c r="A157" t="n">
@@ -6409,6 +7349,12 @@
       <c r="L157" t="n">
         <v>0.9651587265525744</v>
       </c>
+      <c r="M157" t="n">
+        <v>0.005539613484260969</v>
+      </c>
+      <c r="N157" t="n">
+        <v>0.002739290366066002</v>
+      </c>
     </row>
     <row r="158">
       <c r="A158" t="n">
@@ -6447,6 +7393,12 @@
       <c r="L158" t="n">
         <v>0.8616389037587298</v>
       </c>
+      <c r="M158" t="n">
+        <v>0.001485153170452617</v>
+      </c>
+      <c r="N158" t="n">
+        <v>0.01025885407589104</v>
+      </c>
     </row>
     <row r="159">
       <c r="A159" t="n">
@@ -6485,6 +7437,12 @@
       <c r="L159" t="n">
         <v>0.7512962372181093</v>
       </c>
+      <c r="M159" t="n">
+        <v>0.00127840669982655</v>
+      </c>
+      <c r="N159" t="n">
+        <v>0.0119205015391163</v>
+      </c>
     </row>
     <row r="160">
       <c r="A160" t="n">
@@ -6523,6 +7481,12 @@
       <c r="L160" t="n">
         <v>0.9470837956430446</v>
       </c>
+      <c r="M160" t="n">
+        <v>0.00386974124250449</v>
+      </c>
+      <c r="N160" t="n">
+        <v>0.003927597811145537</v>
+      </c>
     </row>
     <row r="161">
       <c r="A161" t="n">
@@ -6561,6 +7525,12 @@
       <c r="L161" t="n">
         <v>0.857980548293648</v>
       </c>
+      <c r="M161" t="n">
+        <v>0.0008732311338817761</v>
+      </c>
+      <c r="N161" t="n">
+        <v>0.01745854079401101</v>
+      </c>
     </row>
     <row r="162">
       <c r="A162" t="n">
@@ -6599,6 +7569,12 @@
       <c r="L162" t="n">
         <v>0.8658949218634072</v>
       </c>
+      <c r="M162" t="n">
+        <v>0.001229688880730038</v>
+      </c>
+      <c r="N162" t="n">
+        <v>0.01239295914519602</v>
+      </c>
     </row>
     <row r="163">
       <c r="A163" t="n">
@@ -6637,6 +7613,12 @@
       <c r="L163" t="n">
         <v>0.805773390450323</v>
       </c>
+      <c r="M163" t="n">
+        <v>0.001205125796100384</v>
+      </c>
+      <c r="N163" t="n">
+        <v>0.01264646021222788</v>
+      </c>
     </row>
     <row r="164">
       <c r="A164" t="n">
@@ -6675,6 +7657,12 @@
       <c r="L164" t="n">
         <v>0.8736196871349297</v>
       </c>
+      <c r="M164" t="n">
+        <v>0.001366326266343963</v>
+      </c>
+      <c r="N164" t="n">
+        <v>0.01115120573300884</v>
+      </c>
     </row>
     <row r="165">
       <c r="A165" t="n">
@@ -6713,6 +7701,12 @@
       <c r="L165" t="n">
         <v>0.939108484069162</v>
       </c>
+      <c r="M165" t="n">
+        <v>0.002285311732877898</v>
+      </c>
+      <c r="N165" t="n">
+        <v>0.006662058202071442</v>
+      </c>
     </row>
     <row r="166">
       <c r="A166" t="n">
@@ -6751,6 +7745,12 @@
       <c r="L166" t="n">
         <v>0.9906405977737858</v>
       </c>
+      <c r="M166" t="n">
+        <v>0.03296888386925655</v>
+      </c>
+      <c r="N166" t="n">
+        <v>0.0004474985520314226</v>
+      </c>
     </row>
     <row r="167">
       <c r="A167" t="n">
@@ -6789,6 +7789,12 @@
       <c r="L167" t="n">
         <v>0.8530826116568573</v>
       </c>
+      <c r="M167" t="n">
+        <v>0.001437886727565229</v>
+      </c>
+      <c r="N167" t="n">
+        <v>0.01059680611719777</v>
+      </c>
     </row>
     <row r="168">
       <c r="A168" t="n">
@@ -6827,6 +7833,12 @@
       <c r="L168" t="n">
         <v>0.9722263786879105</v>
       </c>
+      <c r="M168" t="n">
+        <v>0.004993463059176256</v>
+      </c>
+      <c r="N168" t="n">
+        <v>0.00304013039714448</v>
+      </c>
     </row>
     <row r="169">
       <c r="A169" t="n">
@@ -6865,6 +7877,12 @@
       <c r="L169" t="n">
         <v>0.9484934364988061</v>
       </c>
+      <c r="M169" t="n">
+        <v>0.0034859617152454</v>
+      </c>
+      <c r="N169" t="n">
+        <v>0.004362045016217803</v>
+      </c>
     </row>
     <row r="170">
       <c r="A170" t="n">
@@ -6903,6 +7921,12 @@
       <c r="L170" t="n">
         <v>0.9925783843171168</v>
       </c>
+      <c r="M170" t="n">
+        <v>0.04755328671187738</v>
+      </c>
+      <c r="N170" t="n">
+        <v>0.0003059847896072909</v>
+      </c>
     </row>
     <row r="171">
       <c r="A171" t="n">
@@ -6941,6 +7965,12 @@
       <c r="L171" t="n">
         <v>0.9685545436579687</v>
       </c>
+      <c r="M171" t="n">
+        <v>0.006148328852298591</v>
+      </c>
+      <c r="N171" t="n">
+        <v>0.002465693573855932</v>
+      </c>
     </row>
     <row r="172">
       <c r="A172" t="n">
@@ -6979,6 +8009,12 @@
       <c r="L172" t="n">
         <v>0.9563516485451775</v>
       </c>
+      <c r="M172" t="n">
+        <v>0.002120109296140735</v>
+      </c>
+      <c r="N172" t="n">
+        <v>0.007181231724152035</v>
+      </c>
     </row>
     <row r="173">
       <c r="A173" t="n">
@@ -7017,6 +8053,12 @@
       <c r="L173" t="n">
         <v>0.9540008309220129</v>
       </c>
+      <c r="M173" t="n">
+        <v>0.009227520794871352</v>
+      </c>
+      <c r="N173" t="n">
+        <v>0.001638612405338634</v>
+      </c>
     </row>
     <row r="174">
       <c r="A174" t="n">
@@ -7055,6 +8097,12 @@
       <c r="L174" t="n">
         <v>0.9625626701757448</v>
       </c>
+      <c r="M174" t="n">
+        <v>0.007645210236561971</v>
+      </c>
+      <c r="N174" t="n">
+        <v>0.001980819862661042</v>
+      </c>
     </row>
     <row r="175">
       <c r="A175" t="n">
@@ -7093,6 +8141,12 @@
       <c r="L175" t="n">
         <v>0.9667779771687682</v>
       </c>
+      <c r="M175" t="n">
+        <v>0.01212732054534083</v>
+      </c>
+      <c r="N175" t="n">
+        <v>0.001243294811832995</v>
+      </c>
     </row>
     <row r="176">
       <c r="A176" t="n">
@@ -7131,6 +8185,12 @@
       <c r="L176" t="n">
         <v>0.8721697648975297</v>
       </c>
+      <c r="M176" t="n">
+        <v>0.001175669736292536</v>
+      </c>
+      <c r="N176" t="n">
+        <v>0.01297039031419546</v>
+      </c>
     </row>
     <row r="177">
       <c r="A177" t="n">
@@ -7169,6 +8229,12 @@
       <c r="L177" t="n">
         <v>0.8788522098760388</v>
       </c>
+      <c r="M177" t="n">
+        <v>0.001447632893026275</v>
+      </c>
+      <c r="N177" t="n">
+        <v>0.01052497172429198</v>
+      </c>
     </row>
     <row r="178">
       <c r="A178" t="n">
@@ -7207,6 +8273,12 @@
       <c r="L178" t="n">
         <v>0.8703968069794688</v>
       </c>
+      <c r="M178" t="n">
+        <v>0.001484329192812877</v>
+      </c>
+      <c r="N178" t="n">
+        <v>0.01026445270730458</v>
+      </c>
     </row>
     <row r="179">
       <c r="A179" t="n">
@@ -7245,6 +8317,12 @@
       <c r="L179" t="n">
         <v>0.8487407540654364</v>
       </c>
+      <c r="M179" t="n">
+        <v>0.0005874375972823765</v>
+      </c>
+      <c r="N179" t="n">
+        <v>0.02596396446021425</v>
+      </c>
     </row>
     <row r="180">
       <c r="A180" t="n">
@@ -7283,6 +8361,12 @@
       <c r="L180" t="n">
         <v>0.7761174041642795</v>
       </c>
+      <c r="M180" t="n">
+        <v>0.001009039904006643</v>
+      </c>
+      <c r="N180" t="n">
+        <v>0.01510643862775086</v>
+      </c>
     </row>
     <row r="181">
       <c r="A181" t="n">
@@ -7321,6 +8405,12 @@
       <c r="L181" t="n">
         <v>0.8954286618736692</v>
       </c>
+      <c r="M181" t="n">
+        <v>0.001918086542186989</v>
+      </c>
+      <c r="N181" t="n">
+        <v>0.007941958483298529</v>
+      </c>
     </row>
     <row r="182">
       <c r="A182" t="n">
@@ -7359,6 +8449,12 @@
       <c r="L182" t="n">
         <v>0.9302450372079671</v>
       </c>
+      <c r="M182" t="n">
+        <v>0.002386193061982818</v>
+      </c>
+      <c r="N182" t="n">
+        <v>0.006379423419909494</v>
+      </c>
     </row>
     <row r="183">
       <c r="A183" t="n">
@@ -7397,6 +8493,12 @@
       <c r="L183" t="n">
         <v>0.9447925145349795</v>
       </c>
+      <c r="M183" t="n">
+        <v>0.007359059952315717</v>
+      </c>
+      <c r="N183" t="n">
+        <v>0.002058401692820507</v>
+      </c>
     </row>
     <row r="184">
       <c r="A184" t="n">
@@ -7435,6 +8537,12 @@
       <c r="L184" t="n">
         <v>0.9109838414475947</v>
       </c>
+      <c r="M184" t="n">
+        <v>0.002449446424235357</v>
+      </c>
+      <c r="N184" t="n">
+        <v>0.006214476054386078</v>
+      </c>
     </row>
     <row r="185">
       <c r="A185" t="n">
@@ -7473,6 +8581,12 @@
       <c r="L185" t="n">
         <v>0.9489132729141622</v>
       </c>
+      <c r="M185" t="n">
+        <v>0.002181217777551635</v>
+      </c>
+      <c r="N185" t="n">
+        <v>0.006980534032494208</v>
+      </c>
     </row>
     <row r="186">
       <c r="A186" t="n">
@@ -7511,6 +8625,12 @@
       <c r="L186" t="n">
         <v>0.7968406198529824</v>
       </c>
+      <c r="M186" t="n">
+        <v>0.001006420420120982</v>
+      </c>
+      <c r="N186" t="n">
+        <v>0.01514598868566722</v>
+      </c>
     </row>
     <row r="187">
       <c r="A187" t="n">
@@ -7549,6 +8669,12 @@
       <c r="L187" t="n">
         <v>0.9516918749727046</v>
       </c>
+      <c r="M187" t="n">
+        <v>0.002236612405237871</v>
+      </c>
+      <c r="N187" t="n">
+        <v>0.006807115110054882</v>
+      </c>
     </row>
     <row r="188">
       <c r="A188" t="n">
@@ -7587,6 +8713,12 @@
       <c r="L188" t="n">
         <v>0.7790191180526161</v>
       </c>
+      <c r="M188" t="n">
+        <v>0.0008226061731488833</v>
+      </c>
+      <c r="N188" t="n">
+        <v>0.01853375507850216</v>
+      </c>
     </row>
     <row r="189">
       <c r="A189" t="n">
@@ -7625,6 +8757,12 @@
       <c r="L189" t="n">
         <v>0.7671983482918699</v>
       </c>
+      <c r="M189" t="n">
+        <v>0.0009550835804456303</v>
+      </c>
+      <c r="N189" t="n">
+        <v>0.01596126932993113</v>
+      </c>
     </row>
     <row r="190">
       <c r="A190" t="n">
@@ -7663,6 +8801,12 @@
       <c r="L190" t="n">
         <v>0.6872440611066247</v>
       </c>
+      <c r="M190" t="n">
+        <v>0.004247101809749691</v>
+      </c>
+      <c r="N190" t="n">
+        <v>0.003577814555362795</v>
+      </c>
     </row>
     <row r="191">
       <c r="A191" t="n">
@@ -7701,6 +8845,12 @@
       <c r="L191" t="n">
         <v>0.9600542711033738</v>
       </c>
+      <c r="M191" t="n">
+        <v>0.002553699982585096</v>
+      </c>
+      <c r="N191" t="n">
+        <v>0.005958600098987621</v>
+      </c>
     </row>
     <row r="192">
       <c r="A192" t="n">
@@ -7739,6 +8889,12 @@
       <c r="L192" t="n">
         <v>0.9754633387549456</v>
       </c>
+      <c r="M192" t="n">
+        <v>0.007687379972977203</v>
+      </c>
+      <c r="N192" t="n">
+        <v>0.001969885476923955</v>
+      </c>
     </row>
     <row r="193">
       <c r="A193" t="n">
@@ -7777,6 +8933,12 @@
       <c r="L193" t="n">
         <v>0.9813908367081372</v>
       </c>
+      <c r="M193" t="n">
+        <v>0.007682023756326685</v>
+      </c>
+      <c r="N193" t="n">
+        <v>0.001970778521836399</v>
+      </c>
     </row>
     <row r="194">
       <c r="A194" t="n">
@@ -7815,6 +8977,12 @@
       <c r="L194" t="n">
         <v>0.9403832706317471</v>
       </c>
+      <c r="M194" t="n">
+        <v>0.001523977576390769</v>
+      </c>
+      <c r="N194" t="n">
+        <v>0.009995197066972774</v>
+      </c>
     </row>
     <row r="195">
       <c r="A195" t="n">
@@ -7853,6 +9021,12 @@
       <c r="L195" t="n">
         <v>0.8170728998343083</v>
       </c>
+      <c r="M195" t="n">
+        <v>0.001250218951999633</v>
+      </c>
+      <c r="N195" t="n">
+        <v>0.01218962777443216</v>
+      </c>
     </row>
     <row r="196">
       <c r="A196" t="n">
@@ -7891,6 +9065,12 @@
       <c r="L196" t="n">
         <v>0.9939196336275143</v>
       </c>
+      <c r="M196" t="n">
+        <v>0.0323893867396039</v>
+      </c>
+      <c r="N196" t="n">
+        <v>0.0004564122110891691</v>
+      </c>
     </row>
     <row r="197">
       <c r="A197" t="n">
@@ -7929,6 +9109,12 @@
       <c r="L197" t="n">
         <v>0.891732917640208</v>
       </c>
+      <c r="M197" t="n">
+        <v>0.002109245776334141</v>
+      </c>
+      <c r="N197" t="n">
+        <v>0.007226830775384397</v>
+      </c>
     </row>
     <row r="198">
       <c r="A198" t="n">
@@ -7967,6 +9153,12 @@
       <c r="L198" t="n">
         <v>0.9930663009677764</v>
       </c>
+      <c r="M198" t="n">
+        <v>0.03290319902290405</v>
+      </c>
+      <c r="N198" t="n">
+        <v>0.0004488966107849707</v>
+      </c>
     </row>
     <row r="199">
       <c r="A199" t="n">
@@ -8005,6 +9197,12 @@
       <c r="L199" t="n">
         <v>0.919967638081108</v>
       </c>
+      <c r="M199" t="n">
+        <v>0.008732791965005668</v>
+      </c>
+      <c r="N199" t="n">
+        <v>0.001732387384245805</v>
+      </c>
     </row>
     <row r="200">
       <c r="A200" t="n">
@@ -8043,6 +9241,12 @@
       <c r="L200" t="n">
         <v>0.9275312704055384</v>
       </c>
+      <c r="M200" t="n">
+        <v>0.002315177492836479</v>
+      </c>
+      <c r="N200" t="n">
+        <v>0.006575796474895652</v>
+      </c>
     </row>
     <row r="201">
       <c r="A201" t="n">
@@ -8081,6 +9285,12 @@
       <c r="L201" t="n">
         <v>0.9682711804086869</v>
       </c>
+      <c r="M201" t="n">
+        <v>0.002379824143660965</v>
+      </c>
+      <c r="N201" t="n">
+        <v>0.006396227700260541</v>
+      </c>
     </row>
     <row r="202">
       <c r="A202" t="n">
@@ -8119,6 +9329,12 @@
       <c r="L202" t="n">
         <v>0.7287952728619775</v>
       </c>
+      <c r="M202" t="n">
+        <v>0.004156517275877005</v>
+      </c>
+      <c r="N202" t="n">
+        <v>0.00365612005820997</v>
+      </c>
     </row>
     <row r="203">
       <c r="A203" t="n">
@@ -8157,6 +9373,12 @@
       <c r="L203" t="n">
         <v>0.7735589314591607</v>
       </c>
+      <c r="M203" t="n">
+        <v>0.00144560398047807</v>
+      </c>
+      <c r="N203" t="n">
+        <v>0.01054025723699513</v>
+      </c>
     </row>
     <row r="204">
       <c r="A204" t="n">
@@ -8195,6 +9417,12 @@
       <c r="L204" t="n">
         <v>0.9148945613626041</v>
       </c>
+      <c r="M204" t="n">
+        <v>0.001656166280790106</v>
+      </c>
+      <c r="N204" t="n">
+        <v>0.009199845460266797</v>
+      </c>
     </row>
     <row r="205">
       <c r="A205" t="n">
@@ -8233,6 +9461,12 @@
       <c r="L205" t="n">
         <v>0.7763660612532213</v>
       </c>
+      <c r="M205" t="n">
+        <v>0.0006968898489640785</v>
+      </c>
+      <c r="N205" t="n">
+        <v>0.02188013511475338</v>
+      </c>
     </row>
     <row r="206">
       <c r="A206" t="n">
@@ -8271,6 +9505,12 @@
       <c r="L206" t="n">
         <v>0.8021122757927752</v>
       </c>
+      <c r="M206" t="n">
+        <v>0.001230962907710061</v>
+      </c>
+      <c r="N206" t="n">
+        <v>0.01238070734867863</v>
+      </c>
     </row>
     <row r="207">
       <c r="A207" t="n">
@@ -8309,6 +9549,12 @@
       <c r="L207" t="n">
         <v>0.923886269178179</v>
       </c>
+      <c r="M207" t="n">
+        <v>0.001390820479924122</v>
+      </c>
+      <c r="N207" t="n">
+        <v>0.01095586527942084</v>
+      </c>
     </row>
     <row r="208">
       <c r="A208" t="n">
@@ -8347,6 +9593,12 @@
       <c r="L208" t="n">
         <v>0.6092333685187826</v>
       </c>
+      <c r="M208" t="n">
+        <v>0.0009200351281511877</v>
+      </c>
+      <c r="N208" t="n">
+        <v>0.01657081874835805</v>
+      </c>
     </row>
     <row r="209">
       <c r="A209" t="n">
@@ -8385,6 +9637,12 @@
       <c r="L209" t="n">
         <v>0.9464388923471249</v>
       </c>
+      <c r="M209" t="n">
+        <v>0.002309771729876189</v>
+      </c>
+      <c r="N209" t="n">
+        <v>0.006591324373558366</v>
+      </c>
     </row>
     <row r="210">
       <c r="A210" t="n">
@@ -8423,6 +9681,12 @@
       <c r="L210" t="n">
         <v>0.898770971588798</v>
       </c>
+      <c r="M210" t="n">
+        <v>0.00876602871663365</v>
+      </c>
+      <c r="N210" t="n">
+        <v>0.001725683987745067</v>
+      </c>
     </row>
     <row r="211">
       <c r="A211" t="n">
@@ -8461,6 +9725,12 @@
       <c r="L211" t="n">
         <v>0.8818298514316694</v>
       </c>
+      <c r="M211" t="n">
+        <v>0.001068533700785016</v>
+      </c>
+      <c r="N211" t="n">
+        <v>0.01426671907007809</v>
+      </c>
     </row>
     <row r="212">
       <c r="A212" t="n">
@@ -8499,6 +9769,12 @@
       <c r="L212" t="n">
         <v>0.9088439636231668</v>
       </c>
+      <c r="M212" t="n">
+        <v>0.005680160946633126</v>
+      </c>
+      <c r="N212" t="n">
+        <v>0.002671188128072309</v>
+      </c>
     </row>
     <row r="213">
       <c r="A213" t="n">
@@ -8537,6 +9813,12 @@
       <c r="L213" t="n">
         <v>0.8602364922524015</v>
       </c>
+      <c r="M213" t="n">
+        <v>0.001613952357369299</v>
+      </c>
+      <c r="N213" t="n">
+        <v>0.009439223649317556</v>
+      </c>
     </row>
     <row r="214">
       <c r="A214" t="n">
@@ -8575,6 +9857,12 @@
       <c r="L214" t="n">
         <v>0.7020197941950117</v>
       </c>
+      <c r="M214" t="n">
+        <v>0.0005309244543841414</v>
+      </c>
+      <c r="N214" t="n">
+        <v>0.02872490902346448</v>
+      </c>
     </row>
     <row r="215">
       <c r="A215" t="n">
@@ -8613,6 +9901,12 @@
       <c r="L215" t="n">
         <v>0.9457878850595735</v>
       </c>
+      <c r="M215" t="n">
+        <v>0.008160380776267507</v>
+      </c>
+      <c r="N215" t="n">
+        <v>0.001854704059531532</v>
+      </c>
     </row>
     <row r="216">
       <c r="A216" t="n">
@@ -8651,6 +9945,12 @@
       <c r="L216" t="n">
         <v>0.85919546694682</v>
       </c>
+      <c r="M216" t="n">
+        <v>0.001139222387505979</v>
+      </c>
+      <c r="N216" t="n">
+        <v>0.01337843441489979</v>
+      </c>
     </row>
     <row r="217">
       <c r="A217" t="n">
@@ -8689,6 +9989,12 @@
       <c r="L217" t="n">
         <v>0.8469608705377366</v>
       </c>
+      <c r="M217" t="n">
+        <v>0.001206039447264911</v>
+      </c>
+      <c r="N217" t="n">
+        <v>0.01263851166848539</v>
+      </c>
     </row>
     <row r="218">
       <c r="A218" t="n">
@@ -8727,6 +10033,12 @@
       <c r="L218" t="n">
         <v>0.9494350658845931</v>
       </c>
+      <c r="M218" t="n">
+        <v>0.002978111536231457</v>
+      </c>
+      <c r="N218" t="n">
+        <v>0.005104281582161699</v>
+      </c>
     </row>
     <row r="219">
       <c r="A219" t="n">
@@ -8765,6 +10077,12 @@
       <c r="L219" t="n">
         <v>0.5434939948840281</v>
       </c>
+      <c r="M219" t="n">
+        <v>0.001993219284174238</v>
+      </c>
+      <c r="N219" t="n">
+        <v>0.007640333102782563</v>
+      </c>
     </row>
     <row r="220">
       <c r="A220" t="n">
@@ -8803,6 +10121,12 @@
       <c r="L220" t="n">
         <v>0.9854049914784433</v>
       </c>
+      <c r="M220" t="n">
+        <v>0.01577461091084626</v>
+      </c>
+      <c r="N220" t="n">
+        <v>0.0009523410766297053</v>
+      </c>
     </row>
     <row r="221">
       <c r="A221" t="n">
@@ -8841,6 +10165,12 @@
       <c r="L221" t="n">
         <v>0.7069036898209576</v>
       </c>
+      <c r="M221" t="n">
+        <v>0.0005638362752745797</v>
+      </c>
+      <c r="N221" t="n">
+        <v>0.02704729979334314</v>
+      </c>
     </row>
     <row r="222">
       <c r="A222" t="n">
@@ -8879,6 +10209,12 @@
       <c r="L222" t="n">
         <v>0.9312471365493515</v>
       </c>
+      <c r="M222" t="n">
+        <v>0.002124097752759701</v>
+      </c>
+      <c r="N222" t="n">
+        <v>0.007168403075136436</v>
+      </c>
     </row>
     <row r="223">
       <c r="A223" t="n">
@@ -8917,6 +10253,12 @@
       <c r="L223" t="n">
         <v>0.8366856701950376</v>
       </c>
+      <c r="M223" t="n">
+        <v>0.001022882548441924</v>
+      </c>
+      <c r="N223" t="n">
+        <v>0.01490230520614643</v>
+      </c>
     </row>
     <row r="224">
       <c r="A224" t="n">
@@ -8955,6 +10297,12 @@
       <c r="L224" t="n">
         <v>0.7744984700572397</v>
       </c>
+      <c r="M224" t="n">
+        <v>0.0008898473410417412</v>
+      </c>
+      <c r="N224" t="n">
+        <v>0.01713212517613988</v>
+      </c>
     </row>
     <row r="225">
       <c r="A225" t="n">
@@ -8993,6 +10341,12 @@
       <c r="L225" t="n">
         <v>0.9886010378626365</v>
       </c>
+      <c r="M225" t="n">
+        <v>0.02362865190358163</v>
+      </c>
+      <c r="N225" t="n">
+        <v>0.0006307638340845549</v>
+      </c>
     </row>
     <row r="226">
       <c r="A226" t="n">
@@ -9031,6 +10385,12 @@
       <c r="L226" t="n">
         <v>0.9281965555980733</v>
       </c>
+      <c r="M226" t="n">
+        <v>0.002257754562468475</v>
+      </c>
+      <c r="N226" t="n">
+        <v>0.006743062538843529</v>
+      </c>
     </row>
     <row r="227">
       <c r="A227" t="n">
@@ -9069,6 +10429,12 @@
       <c r="L227" t="n">
         <v>0.8975644112940979</v>
       </c>
+      <c r="M227" t="n">
+        <v>0.001564716704072065</v>
+      </c>
+      <c r="N227" t="n">
+        <v>0.009734955358271362</v>
+      </c>
     </row>
     <row r="228">
       <c r="A228" t="n">
@@ -9107,6 +10473,12 @@
       <c r="L228" t="n">
         <v>0.8126716311475635</v>
       </c>
+      <c r="M228" t="n">
+        <v>0.0008648089986412377</v>
+      </c>
+      <c r="N228" t="n">
+        <v>0.01762859074886199</v>
+      </c>
     </row>
     <row r="229">
       <c r="A229" t="n">
@@ -9145,6 +10517,12 @@
       <c r="L229" t="n">
         <v>0.8656402250178957</v>
       </c>
+      <c r="M229" t="n">
+        <v>0.001107754030505773</v>
+      </c>
+      <c r="N229" t="n">
+        <v>0.01375936899011935</v>
+      </c>
     </row>
     <row r="230">
       <c r="A230" t="n">
@@ -9183,6 +10561,12 @@
       <c r="L230" t="n">
         <v>0.9559941225871927</v>
       </c>
+      <c r="M230" t="n">
+        <v>0.002222747132726445</v>
+      </c>
+      <c r="N230" t="n">
+        <v>0.006849819561838961</v>
+      </c>
     </row>
     <row r="231">
       <c r="A231" t="n">
@@ -9221,6 +10605,12 @@
       <c r="L231" t="n">
         <v>0.952359592197132</v>
       </c>
+      <c r="M231" t="n">
+        <v>0.007124220870528234</v>
+      </c>
+      <c r="N231" t="n">
+        <v>0.002126681901044035</v>
+      </c>
     </row>
     <row r="232">
       <c r="A232" t="n">
@@ -9259,6 +10649,12 @@
       <c r="L232" t="n">
         <v>0.9275589919767505</v>
       </c>
+      <c r="M232" t="n">
+        <v>0.002316015069087365</v>
+      </c>
+      <c r="N232" t="n">
+        <v>0.006573412552334853</v>
+      </c>
     </row>
     <row r="233">
       <c r="A233" t="n">
@@ -9297,6 +10693,12 @@
       <c r="L233" t="n">
         <v>0.7926315435684637</v>
       </c>
+      <c r="M233" t="n">
+        <v>0.004468484224812728</v>
+      </c>
+      <c r="N233" t="n">
+        <v>0.003399759683627686</v>
+      </c>
     </row>
     <row r="234">
       <c r="A234" t="n">
@@ -9335,6 +10737,12 @@
       <c r="L234" t="n">
         <v>0.8111142932347496</v>
       </c>
+      <c r="M234" t="n">
+        <v>0.001336166074133207</v>
+      </c>
+      <c r="N234" t="n">
+        <v>0.01140454537358374</v>
+      </c>
     </row>
     <row r="235">
       <c r="A235" t="n">
@@ -9373,6 +10781,12 @@
       <c r="L235" t="n">
         <v>0.9938065150516396</v>
       </c>
+      <c r="M235" t="n">
+        <v>0.06523623811437017</v>
+      </c>
+      <c r="N235" t="n">
+        <v>0.0002191888177441559</v>
+      </c>
     </row>
     <row r="236">
       <c r="A236" t="n">
@@ -9411,6 +10825,12 @@
       <c r="L236" t="n">
         <v>0.9965046005806635</v>
       </c>
+      <c r="M236" t="n">
+        <v>0.06566021653178143</v>
+      </c>
+      <c r="N236" t="n">
+        <v>0.0002171440124876943</v>
+      </c>
     </row>
     <row r="237">
       <c r="A237" t="n">
@@ -9449,6 +10869,12 @@
       <c r="L237" t="n">
         <v>0.9605621619887066</v>
       </c>
+      <c r="M237" t="n">
+        <v>0.01512918569388445</v>
+      </c>
+      <c r="N237" t="n">
+        <v>0.0009936949495986671</v>
+      </c>
     </row>
     <row r="238">
       <c r="A238" t="n">
@@ -9487,6 +10913,12 @@
       <c r="L238" t="n">
         <v>0.9595258432183922</v>
       </c>
+      <c r="M238" t="n">
+        <v>0.006180479594192633</v>
+      </c>
+      <c r="N238" t="n">
+        <v>0.0024533556736841</v>
+      </c>
     </row>
     <row r="239">
       <c r="A239" t="n">
@@ -9525,6 +10957,12 @@
       <c r="L239" t="n">
         <v>0.9714983059999561</v>
       </c>
+      <c r="M239" t="n">
+        <v>0.01063166367239064</v>
+      </c>
+      <c r="N239" t="n">
+        <v>0.001420233438492555</v>
+      </c>
     </row>
     <row r="240">
       <c r="A240" t="n">
@@ -9563,6 +11001,12 @@
       <c r="L240" t="n">
         <v>0.9274602155728391</v>
       </c>
+      <c r="M240" t="n">
+        <v>0.001365835066874943</v>
+      </c>
+      <c r="N240" t="n">
+        <v>0.01116072101357383</v>
+      </c>
     </row>
     <row r="241">
       <c r="A241" t="n">
@@ -9601,6 +11045,12 @@
       <c r="L241" t="n">
         <v>0.9085921252295469</v>
       </c>
+      <c r="M241" t="n">
+        <v>0.001991676416607331</v>
+      </c>
+      <c r="N241" t="n">
+        <v>0.007646230508697601</v>
+      </c>
     </row>
     <row r="242">
       <c r="A242" t="n">
@@ -9639,6 +11089,12 @@
       <c r="L242" t="n">
         <v>0.9887052526383721</v>
       </c>
+      <c r="M242" t="n">
+        <v>0.02762306988096747</v>
+      </c>
+      <c r="N242" t="n">
+        <v>0.0005374297664329978</v>
+      </c>
     </row>
     <row r="243">
       <c r="A243" t="n">
@@ -9677,6 +11133,12 @@
       <c r="L243" t="n">
         <v>0.9111331220875103</v>
       </c>
+      <c r="M243" t="n">
+        <v>0.006024206744471301</v>
+      </c>
+      <c r="N243" t="n">
+        <v>0.002517823648640098</v>
+      </c>
     </row>
     <row r="244">
       <c r="A244" t="n">
@@ -9715,6 +11177,12 @@
       <c r="L244" t="n">
         <v>0.6518551054404316</v>
       </c>
+      <c r="M244" t="n">
+        <v>0.0006458132902721795</v>
+      </c>
+      <c r="N244" t="n">
+        <v>0.02361210253777147</v>
+      </c>
     </row>
     <row r="245">
       <c r="A245" t="n">
@@ -9753,6 +11221,12 @@
       <c r="L245" t="n">
         <v>0.8555437299943502</v>
       </c>
+      <c r="M245" t="n">
+        <v>0.001455125560745628</v>
+      </c>
+      <c r="N245" t="n">
+        <v>0.01047026774287439</v>
+      </c>
     </row>
     <row r="246">
       <c r="A246" t="n">
@@ -9791,6 +11265,12 @@
       <c r="L246" t="n">
         <v>0.8865704326074122</v>
       </c>
+      <c r="M246" t="n">
+        <v>0.001243375252845273</v>
+      </c>
+      <c r="N246" t="n">
+        <v>0.01225677726728006</v>
+      </c>
     </row>
     <row r="247">
       <c r="A247" t="n">
@@ -9829,6 +11309,12 @@
       <c r="L247" t="n">
         <v>0.9252432371210543</v>
       </c>
+      <c r="M247" t="n">
+        <v>0.004011182649266124</v>
+      </c>
+      <c r="N247" t="n">
+        <v>0.003789037555407466</v>
+      </c>
     </row>
     <row r="248">
       <c r="A248" t="n">
@@ -9867,6 +11353,12 @@
       <c r="L248" t="n">
         <v>0.7968808057757981</v>
       </c>
+      <c r="M248" t="n">
+        <v>0.001006675418918831</v>
+      </c>
+      <c r="N248" t="n">
+        <v>0.01514214827659404</v>
+      </c>
     </row>
     <row r="249">
       <c r="A249" t="n">
@@ -9905,6 +11397,12 @@
       <c r="L249" t="n">
         <v>0.7863615956273168</v>
       </c>
+      <c r="M249" t="n">
+        <v>0.0008874712734840242</v>
+      </c>
+      <c r="N249" t="n">
+        <v>0.01717748101125731</v>
+      </c>
     </row>
     <row r="250">
       <c r="A250" t="n">
@@ -9943,6 +11441,12 @@
       <c r="L250" t="n">
         <v>0.7960439233613026</v>
       </c>
+      <c r="M250" t="n">
+        <v>0.0009902232832735022</v>
+      </c>
+      <c r="N250" t="n">
+        <v>0.01539399774506279</v>
+      </c>
     </row>
     <row r="251">
       <c r="A251" t="n">
@@ -9981,6 +11485,12 @@
       <c r="L251" t="n">
         <v>0.824208606551422</v>
       </c>
+      <c r="M251" t="n">
+        <v>0.001110869338471518</v>
+      </c>
+      <c r="N251" t="n">
+        <v>0.01372067759050538</v>
+      </c>
     </row>
     <row r="252">
       <c r="A252" t="n">
@@ -10019,6 +11529,12 @@
       <c r="L252" t="n">
         <v>0.9849939562411525</v>
       </c>
+      <c r="M252" t="n">
+        <v>0.02636554710166245</v>
+      </c>
+      <c r="N252" t="n">
+        <v>0.0005632437814867804</v>
+      </c>
     </row>
     <row r="253">
       <c r="A253" t="n">
@@ -10057,6 +11573,12 @@
       <c r="L253" t="n">
         <v>0.8790787104443337</v>
       </c>
+      <c r="M253" t="n">
+        <v>0.001244244664555028</v>
+      </c>
+      <c r="N253" t="n">
+        <v>0.01224833512858132</v>
+      </c>
     </row>
     <row r="254">
       <c r="A254" t="n">
@@ -10095,6 +11617,12 @@
       <c r="L254" t="n">
         <v>0.9053258334641037</v>
       </c>
+      <c r="M254" t="n">
+        <v>0.001328770102896253</v>
+      </c>
+      <c r="N254" t="n">
+        <v>0.01146739584102336</v>
+      </c>
     </row>
     <row r="255">
       <c r="A255" t="n">
@@ -10133,6 +11661,12 @@
       <c r="L255" t="n">
         <v>0.9465411481176264</v>
       </c>
+      <c r="M255" t="n">
+        <v>0.002310200212606547</v>
+      </c>
+      <c r="N255" t="n">
+        <v>0.006590110148338659</v>
+      </c>
     </row>
     <row r="256">
       <c r="A256" t="n">
@@ -10171,6 +11705,12 @@
       <c r="L256" t="n">
         <v>0.9211912058595105</v>
       </c>
+      <c r="M256" t="n">
+        <v>0.00164959956636285</v>
+      </c>
+      <c r="N256" t="n">
+        <v>0.009234729997000181</v>
+      </c>
     </row>
     <row r="257">
       <c r="A257" t="n">
@@ -10209,6 +11749,12 @@
       <c r="L257" t="n">
         <v>0.9913376787335562</v>
       </c>
+      <c r="M257" t="n">
+        <v>0.02179781368855471</v>
+      </c>
+      <c r="N257" t="n">
+        <v>0.0006848848809626688</v>
+      </c>
     </row>
     <row r="258">
       <c r="A258" t="n">
@@ -10247,6 +11793,12 @@
       <c r="L258" t="n">
         <v>0.8787817685588221</v>
       </c>
+      <c r="M258" t="n">
+        <v>0.001447437491021912</v>
+      </c>
+      <c r="N258" t="n">
+        <v>0.01052639716085346</v>
+      </c>
     </row>
     <row r="259">
       <c r="A259" t="n">
@@ -10285,6 +11837,12 @@
       <c r="L259" t="n">
         <v>0.8378367664299383</v>
       </c>
+      <c r="M259" t="n">
+        <v>0.0008334085221627642</v>
+      </c>
+      <c r="N259" t="n">
+        <v>0.01829547402869676</v>
+      </c>
     </row>
     <row r="260">
       <c r="A260" t="n">
@@ -10323,6 +11881,12 @@
       <c r="L260" t="n">
         <v>0.9775228841346357</v>
       </c>
+      <c r="M260" t="n">
+        <v>0.01104288135418783</v>
+      </c>
+      <c r="N260" t="n">
+        <v>0.001366857870960639</v>
+      </c>
     </row>
     <row r="261">
       <c r="A261" t="n">
@@ -10361,6 +11925,12 @@
       <c r="L261" t="n">
         <v>0.9273620830427617</v>
       </c>
+      <c r="M261" t="n">
+        <v>0.003113538275890325</v>
+      </c>
+      <c r="N261" t="n">
+        <v>0.004885700173168996</v>
+      </c>
     </row>
     <row r="262">
       <c r="A262" t="n">
@@ -10399,6 +11969,12 @@
       <c r="L262" t="n">
         <v>0.9403334298306244</v>
       </c>
+      <c r="M262" t="n">
+        <v>0.002470058814441758</v>
+      </c>
+      <c r="N262" t="n">
+        <v>0.006159799436403755</v>
+      </c>
     </row>
     <row r="263">
       <c r="A263" t="n">
@@ -10437,6 +12013,12 @@
       <c r="L263" t="n">
         <v>0.9561945731731439</v>
       </c>
+      <c r="M263" t="n">
+        <v>0.002117476022048199</v>
+      </c>
+      <c r="N263" t="n">
+        <v>0.007190167557835574</v>
+      </c>
     </row>
     <row r="264">
       <c r="A264" t="n">
@@ -10475,6 +12057,12 @@
       <c r="L264" t="n">
         <v>0.9247865822233969</v>
       </c>
+      <c r="M264" t="n">
+        <v>0.009103682186106221</v>
+      </c>
+      <c r="N264" t="n">
+        <v>0.001661225233061589</v>
+      </c>
     </row>
     <row r="265">
       <c r="A265" t="n">
@@ -10513,6 +12101,12 @@
       <c r="L265" t="n">
         <v>0.9009297814520196</v>
       </c>
+      <c r="M265" t="n">
+        <v>0.001645412408688457</v>
+      </c>
+      <c r="N265" t="n">
+        <v>0.009257895198691119</v>
+      </c>
     </row>
     <row r="266">
       <c r="A266" t="n">
@@ -10551,6 +12145,12 @@
       <c r="L266" t="n">
         <v>0.945441546187052</v>
       </c>
+      <c r="M266" t="n">
+        <v>0.002219776818494535</v>
+      </c>
+      <c r="N266" t="n">
+        <v>0.006858582016723701</v>
+      </c>
     </row>
     <row r="267">
       <c r="A267" t="n">
@@ -10589,6 +12189,12 @@
       <c r="L267" t="n">
         <v>0.9538794497626429</v>
       </c>
+      <c r="M267" t="n">
+        <v>0.004110997717264735</v>
+      </c>
+      <c r="N267" t="n">
+        <v>0.003696696126643068</v>
+      </c>
     </row>
     <row r="268">
       <c r="A268" t="n">
@@ -10627,6 +12233,12 @@
       <c r="L268" t="n">
         <v>0.8973042975204144</v>
       </c>
+      <c r="M268" t="n">
+        <v>0.001413584707865779</v>
+      </c>
+      <c r="N268" t="n">
+        <v>0.010779059944196</v>
+      </c>
     </row>
     <row r="269">
       <c r="A269" t="n">
@@ -10665,6 +12277,12 @@
       <c r="L269" t="n">
         <v>0.7799306664811679</v>
       </c>
+      <c r="M269" t="n">
+        <v>0.001524923323822545</v>
+      </c>
+      <c r="N269" t="n">
+        <v>0.00999120234875585</v>
+      </c>
     </row>
     <row r="270">
       <c r="A270" t="n">
@@ -10703,6 +12321,12 @@
       <c r="L270" t="n">
         <v>0.9852078319379987</v>
       </c>
+      <c r="M270" t="n">
+        <v>0.01498416449537471</v>
+      </c>
+      <c r="N270" t="n">
+        <v>0.001002831680582738</v>
+      </c>
     </row>
     <row r="271">
       <c r="A271" t="n">
@@ -10741,6 +12365,12 @@
       <c r="L271" t="n">
         <v>0.9902980981105554</v>
       </c>
+      <c r="M271" t="n">
+        <v>0.02447148275595947</v>
+      </c>
+      <c r="N271" t="n">
+        <v>0.0006087438877305301</v>
+      </c>
     </row>
     <row r="272">
       <c r="A272" t="n">
@@ -10779,6 +12409,12 @@
       <c r="L272" t="n">
         <v>0.9239259234239505</v>
       </c>
+      <c r="M272" t="n">
+        <v>0.00139141575542472</v>
+      </c>
+      <c r="N272" t="n">
+        <v>0.0109511739370778</v>
+      </c>
     </row>
     <row r="273">
       <c r="A273" t="n">
@@ -10817,6 +12453,12 @@
       <c r="L273" t="n">
         <v>0.9789543906011339</v>
       </c>
+      <c r="M273" t="n">
+        <v>0.01816622122754851</v>
+      </c>
+      <c r="N273" t="n">
+        <v>0.0008246840992050875</v>
+      </c>
     </row>
     <row r="274">
       <c r="A274" t="n">
@@ -10855,6 +12497,12 @@
       <c r="L274" t="n">
         <v>0.8183329455520688</v>
       </c>
+      <c r="M274" t="n">
+        <v>0.000982085504654539</v>
+      </c>
+      <c r="N274" t="n">
+        <v>0.01551532315249995</v>
+      </c>
     </row>
     <row r="275">
       <c r="A275" t="n">
@@ -10893,6 +12541,12 @@
       <c r="L275" t="n">
         <v>0.9336610431603631</v>
       </c>
+      <c r="M275" t="n">
+        <v>0.005695383349070409</v>
+      </c>
+      <c r="N275" t="n">
+        <v>0.002663938745824776</v>
+      </c>
     </row>
     <row r="276">
       <c r="A276" t="n">
@@ -10931,6 +12585,12 @@
       <c r="L276" t="n">
         <v>0.9261793747827445</v>
       </c>
+      <c r="M276" t="n">
+        <v>0.001976927253926214</v>
+      </c>
+      <c r="N276" t="n">
+        <v>0.007702446198348717</v>
+      </c>
     </row>
     <row r="277">
       <c r="A277" t="n">
@@ -10969,6 +12629,12 @@
       <c r="L277" t="n">
         <v>0.9381941348894683</v>
       </c>
+      <c r="M277" t="n">
+        <v>0.002636678687444955</v>
+      </c>
+      <c r="N277" t="n">
+        <v>0.005772050076956699</v>
+      </c>
     </row>
     <row r="278">
       <c r="A278" t="n">
@@ -11007,6 +12673,12 @@
       <c r="L278" t="n">
         <v>0.9920369214925914</v>
       </c>
+      <c r="M278" t="n">
+        <v>0.03858564224046495</v>
+      </c>
+      <c r="N278" t="n">
+        <v>0.00038004573647997</v>
+      </c>
     </row>
     <row r="279">
       <c r="A279" t="n">
@@ -11045,6 +12717,12 @@
       <c r="L279" t="n">
         <v>0.9193212881701029</v>
       </c>
+      <c r="M279" t="n">
+        <v>0.001755895398615504</v>
+      </c>
+      <c r="N279" t="n">
+        <v>0.008673370282313587</v>
+      </c>
     </row>
     <row r="280">
       <c r="A280" t="n">
@@ -11083,6 +12761,12 @@
       <c r="L280" t="n">
         <v>0.9401272660504705</v>
       </c>
+      <c r="M280" t="n">
+        <v>0.001521759851786166</v>
+      </c>
+      <c r="N280" t="n">
+        <v>0.01000975456081262</v>
+      </c>
     </row>
     <row r="281">
       <c r="A281" t="n">
@@ -11121,6 +12805,12 @@
       <c r="L281" t="n">
         <v>0.9440386228493813</v>
       </c>
+      <c r="M281" t="n">
+        <v>0.001791604345001916</v>
+      </c>
+      <c r="N281" t="n">
+        <v>0.008499165239891769</v>
+      </c>
     </row>
     <row r="282">
       <c r="A282" t="n">
@@ -11159,6 +12849,12 @@
       <c r="L282" t="n">
         <v>0.7767230002237232</v>
       </c>
+      <c r="M282" t="n">
+        <v>0.001083743020125016</v>
+      </c>
+      <c r="N282" t="n">
+        <v>0.01406450743526678</v>
+      </c>
     </row>
     <row r="283">
       <c r="A283" t="n">
@@ -11197,6 +12893,12 @@
       <c r="L283" t="n">
         <v>0.9742169617094989</v>
       </c>
+      <c r="M283" t="n">
+        <v>0.01889393462421233</v>
+      </c>
+      <c r="N283" t="n">
+        <v>0.0007922268022920239</v>
+      </c>
     </row>
     <row r="284">
       <c r="A284" t="n">
@@ -11235,6 +12937,12 @@
       <c r="L284" t="n">
         <v>0.99034949300775</v>
       </c>
+      <c r="M284" t="n">
+        <v>0.01889557364860206</v>
+      </c>
+      <c r="N284" t="n">
+        <v>0.0007926739893226338</v>
+      </c>
     </row>
     <row r="285">
       <c r="A285" t="n">
@@ -11273,6 +12981,12 @@
       <c r="L285" t="n">
         <v>0.7090416073858389</v>
       </c>
+      <c r="M285" t="n">
+        <v>0.0007180930767243703</v>
+      </c>
+      <c r="N285" t="n">
+        <v>0.02123370342371969</v>
+      </c>
     </row>
     <row r="286">
       <c r="A286" t="n">
@@ -11311,6 +13025,12 @@
       <c r="L286" t="n">
         <v>0.7993663473358202</v>
       </c>
+      <c r="M286" t="n">
+        <v>0.0008488550737678924</v>
+      </c>
+      <c r="N286" t="n">
+        <v>0.01796022871465153</v>
+      </c>
     </row>
     <row r="287">
       <c r="A287" t="n">
@@ -11349,6 +13069,12 @@
       <c r="L287" t="n">
         <v>0.9162430623527515</v>
       </c>
+      <c r="M287" t="n">
+        <v>0.008681548484089426</v>
+      </c>
+      <c r="N287" t="n">
+        <v>0.001742677044167095</v>
+      </c>
     </row>
     <row r="288">
       <c r="A288" t="n">
@@ -11387,6 +13113,12 @@
       <c r="L288" t="n">
         <v>0.9794669931149851</v>
       </c>
+      <c r="M288" t="n">
+        <v>0.01172468211085966</v>
+      </c>
+      <c r="N288" t="n">
+        <v>0.001286482301879759</v>
+      </c>
     </row>
     <row r="289">
       <c r="A289" t="n">
@@ -11425,6 +13157,12 @@
       <c r="L289" t="n">
         <v>0.9153659033565343</v>
       </c>
+      <c r="M289" t="n">
+        <v>0.001985360402978721</v>
+      </c>
+      <c r="N289" t="n">
+        <v>0.007670543914297736</v>
+      </c>
     </row>
     <row r="290">
       <c r="A290" t="n">
@@ -11463,6 +13201,12 @@
       <c r="L290" t="n">
         <v>0.9424640731449692</v>
       </c>
+      <c r="M290" t="n">
+        <v>0.005222717454611764</v>
+      </c>
+      <c r="N290" t="n">
+        <v>0.002904377087910603</v>
+      </c>
     </row>
     <row r="291">
       <c r="A291" t="n">
@@ -11501,6 +13245,12 @@
       <c r="L291" t="n">
         <v>0.9510379381651641</v>
       </c>
+      <c r="M291" t="n">
+        <v>0.003607264483667133</v>
+      </c>
+      <c r="N291" t="n">
+        <v>0.00421492895073487</v>
+      </c>
     </row>
     <row r="292">
       <c r="A292" t="n">
@@ -11539,6 +13289,12 @@
       <c r="L292" t="n">
         <v>0.9906481158505182</v>
       </c>
+      <c r="M292" t="n">
+        <v>0.0329312793197608</v>
+      </c>
+      <c r="N292" t="n">
+        <v>0.0004485882913084362</v>
+      </c>
     </row>
     <row r="293">
       <c r="A293" t="n">
@@ -11577,6 +13333,12 @@
       <c r="L293" t="n">
         <v>0.8629776539929117</v>
       </c>
+      <c r="M293" t="n">
+        <v>0.001637158942471817</v>
+      </c>
+      <c r="N293" t="n">
+        <v>0.009305063398087291</v>
+      </c>
     </row>
     <row r="294">
       <c r="A294" t="n">
@@ -11615,6 +13377,12 @@
       <c r="L294" t="n">
         <v>0.9222270436791973</v>
       </c>
+      <c r="M294" t="n">
+        <v>0.002011258899042321</v>
+      </c>
+      <c r="N294" t="n">
+        <v>0.007571071333741366</v>
+      </c>
     </row>
     <row r="295">
       <c r="A295" t="n">
@@ -11653,6 +13421,12 @@
       <c r="L295" t="n">
         <v>0.9455340732602586</v>
       </c>
+      <c r="M295" t="n">
+        <v>0.002316697333640333</v>
+      </c>
+      <c r="N295" t="n">
+        <v>0.006571490376445105</v>
+      </c>
     </row>
     <row r="296">
       <c r="A296" t="n">
@@ -11691,6 +13465,12 @@
       <c r="L296" t="n">
         <v>0.9566016395788159</v>
       </c>
+      <c r="M296" t="n">
+        <v>0.002184304425414937</v>
+      </c>
+      <c r="N296" t="n">
+        <v>0.006977582069451147</v>
+      </c>
     </row>
     <row r="297">
       <c r="A297" t="n">
@@ -11729,6 +13509,12 @@
       <c r="L297" t="n">
         <v>0.894660437114029</v>
       </c>
+      <c r="M297" t="n">
+        <v>0.001518802537354806</v>
+      </c>
+      <c r="N297" t="n">
+        <v>0.01003144862690653</v>
+      </c>
     </row>
     <row r="298">
       <c r="A298" t="n">
@@ -11767,6 +13553,12 @@
       <c r="L298" t="n">
         <v>0.9924149942195647</v>
       </c>
+      <c r="M298" t="n">
+        <v>0.02513684968931745</v>
+      </c>
+      <c r="N298" t="n">
+        <v>0.0005916514932523493</v>
+      </c>
     </row>
     <row r="299">
       <c r="A299" t="n">
@@ -11805,6 +13597,12 @@
       <c r="L299" t="n">
         <v>0.9091696347333994</v>
       </c>
+      <c r="M299" t="n">
+        <v>0.001811305853149126</v>
+      </c>
+      <c r="N299" t="n">
+        <v>0.008408994606621952</v>
+      </c>
     </row>
     <row r="300">
       <c r="A300" t="n">
@@ -11843,6 +13641,12 @@
       <c r="L300" t="n">
         <v>0.8764623865572982</v>
       </c>
+      <c r="M300" t="n">
+        <v>0.003916776419382631</v>
+      </c>
+      <c r="N300" t="n">
+        <v>0.003880562587716014</v>
+      </c>
     </row>
     <row r="301">
       <c r="A301" t="n">
@@ -11880,6 +13684,12 @@
       </c>
       <c r="L301" t="n">
         <v>0.8943485177590624</v>
+      </c>
+      <c r="M301" t="n">
+        <v>0.001252786515073376</v>
+      </c>
+      <c r="N301" t="n">
+        <v>0.01216651240291388</v>
       </c>
     </row>
   </sheetData>

</xml_diff>